<commit_message>
Worked through question 7.
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary van Valkenburg\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athelize\Desktop\NSS Data Analytics\Excel\lookups_exercise-Athelize\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19ED61FC-0AAB-4DAC-83F6-00D6AC42053B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAD9A16-DC2D-497A-A50F-DC33E1383259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="90" windowWidth="21877" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
     <sheet name="data_dictionary" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">metro_budget!$A$1:$P$107</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="90">
   <si>
     <t>Department</t>
   </si>
@@ -314,7 +317,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,7 +461,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -879,6 +882,974 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>metro_budget!$B$87</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>ECC Emergency Comm Center</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$B$82:$B$83</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Department</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Budget</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$87</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$B$84:$B$87</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>14860800</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15309700</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15311800</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EB20-4377-937C-C381A7E5E8FC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$C$82:$C$83</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Department</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$87</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$C$84:$C$87</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>14439480.050000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14645233.51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14346057.039999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EB20-4377-937C-C381A7E5E8FC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1582751279"/>
+        <c:axId val="1582748879"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1582751279"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1582748879"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1582748879"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1582751279"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>747711</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>819149</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BC7E27A-C292-78FB-2C0A-DF0933F79CB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1176,13 +2147,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P107"/>
+  <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88:G93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
@@ -1196,7 +2167,7 @@
     <col min="16" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1246,7 +2217,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1256,23 +2227,56 @@
       <c r="C2">
         <v>341243679.13</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="D2">
+        <f>C2-B2</f>
+        <v>-15396420.870000005</v>
+      </c>
+      <c r="E2" s="5">
+        <f>IF(B2&lt;&gt;0, (C2-B2)/B2, IF(C2=0, 0, ""))</f>
+        <v>-4.3170750765267295E-2</v>
+      </c>
+      <c r="F2">
+        <f>IF(E2&lt;&gt;"", RANK(E2, $E$2:$E$52), "")</f>
+        <v>38</v>
+      </c>
       <c r="G2">
         <v>382685200</v>
       </c>
       <c r="H2">
         <v>346340810.81999999</v>
       </c>
-      <c r="J2" s="5"/>
+      <c r="I2">
+        <f>H2-G2</f>
+        <v>-36344389.180000007</v>
+      </c>
+      <c r="J2" s="5">
+        <f>IF(G2&lt;&gt;0, (H2-G2)/G2, IF(H2=0, 0, ""))</f>
+        <v>-9.4972027086493035E-2</v>
+      </c>
+      <c r="K2">
+        <f>IF(J2&lt;&gt;"", RANK(J2, $J$2:$J$52, 0), "")</f>
+        <v>42</v>
+      </c>
       <c r="L2">
         <v>376548600</v>
       </c>
       <c r="M2">
         <v>355279492.22999901</v>
       </c>
-      <c r="O2" s="5"/>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="N2">
+        <f>M2-L2</f>
+        <v>-21269107.770000994</v>
+      </c>
+      <c r="O2" s="5">
+        <f>IF(L2&lt;&gt;0, (M2-L2)/L2, IF(M2=0, 0, ""))</f>
+        <v>-5.6484362894991494E-2</v>
+      </c>
+      <c r="P2">
+        <f>IF(O2&lt;&gt;"", RANK(O2, $O$2:$O$52), "")</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1282,23 +2286,56 @@
       <c r="C3">
         <v>321214.59000000003</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="D3">
+        <f>C3-B3</f>
+        <v>-7585.4099999999744</v>
+      </c>
+      <c r="E3" s="5">
+        <f>IF(B3&lt;&gt;0, (C3-B3)/B3, IF(C3=0, 0, ""))</f>
+        <v>-2.3069981751824741E-2</v>
+      </c>
+      <c r="F3">
+        <f>IF(E3&lt;&gt;"", RANK(E3, $E$2:$E$52), "")</f>
+        <v>30</v>
+      </c>
       <c r="G3">
         <v>334800</v>
       </c>
       <c r="H3">
         <v>312433.70999999897</v>
       </c>
-      <c r="J3" s="5"/>
+      <c r="I3">
+        <f>H3-G3</f>
+        <v>-22366.290000001027</v>
+      </c>
+      <c r="J3" s="5">
+        <f>IF(G3&lt;&gt;0, (H3-G3)/G3, IF(H3=0, 0, ""))</f>
+        <v>-6.6804928315415249E-2</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K52" si="0">IF(J3&lt;&gt;"", RANK(J3, $J$2:$J$52, 0), "")</f>
+        <v>38</v>
+      </c>
       <c r="L3">
         <v>322700</v>
       </c>
       <c r="M3">
         <v>322263.03999999998</v>
       </c>
-      <c r="O3" s="5"/>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="N3">
+        <f t="shared" ref="N3:N52" si="1">M3-L3</f>
+        <v>-436.96000000002095</v>
+      </c>
+      <c r="O3" s="5">
+        <f t="shared" ref="O3:O52" si="2">IF(L3&lt;&gt;0, (M3-L3)/L3, IF(M3=0, 0, ""))</f>
+        <v>-1.3540749922529313E-3</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P52" si="3">IF(O3&lt;&gt;"", RANK(O3, $O$2:$O$52), "")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1308,23 +2345,56 @@
       <c r="C4">
         <v>3115157.5599999898</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="D4">
+        <f>C4-B4</f>
+        <v>-15442.440000010189</v>
+      </c>
+      <c r="E4" s="5">
+        <f>IF(B4&lt;&gt;0, (C4-B4)/B4, IF(C4=0, 0, ""))</f>
+        <v>-4.9327413275443007E-3</v>
+      </c>
+      <c r="F4">
+        <f>IF(E4&lt;&gt;"", RANK(E4, $E$2:$E$52), "")</f>
+        <v>10</v>
+      </c>
       <c r="G4">
         <v>3652300</v>
       </c>
       <c r="H4">
         <v>3589693.2099999902</v>
       </c>
-      <c r="J4" s="5"/>
+      <c r="I4">
+        <f>H4-G4</f>
+        <v>-62606.790000009816</v>
+      </c>
+      <c r="J4" s="5">
+        <f>IF(G4&lt;&gt;0, (H4-G4)/G4, IF(H4=0, 0, ""))</f>
+        <v>-1.7141743558856015E-2</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
       <c r="L4">
         <v>3662400</v>
       </c>
       <c r="M4">
         <v>3564983.04999999</v>
       </c>
-      <c r="O4" s="5"/>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="N4">
+        <f t="shared" si="1"/>
+        <v>-97416.950000009965</v>
+      </c>
+      <c r="O4" s="5">
+        <f t="shared" si="2"/>
+        <v>-2.6599210899959033E-2</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1334,23 +2404,56 @@
       <c r="C5">
         <v>6947552.6699999999</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="D5">
+        <f>C5-B5</f>
+        <v>-723147.33000000007</v>
+      </c>
+      <c r="E5" s="5">
+        <f>IF(B5&lt;&gt;0, (C5-B5)/B5, IF(C5=0, 0, ""))</f>
+        <v>-9.4273968477453174E-2</v>
+      </c>
+      <c r="F5">
+        <f>IF(E5&lt;&gt;"", RANK(E5, $E$2:$E$52), "")</f>
+        <v>48</v>
+      </c>
       <c r="G5">
         <v>7968300</v>
       </c>
       <c r="H5">
         <v>7020609.3200000003</v>
       </c>
-      <c r="J5" s="5"/>
+      <c r="I5">
+        <f>H5-G5</f>
+        <v>-947690.6799999997</v>
+      </c>
+      <c r="J5" s="5">
+        <f>IF(G5&lt;&gt;0, (H5-G5)/G5, IF(H5=0, 0, ""))</f>
+        <v>-0.118932605449092</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
       <c r="L5">
         <v>7759600</v>
       </c>
       <c r="M5">
         <v>7497322.9100000001</v>
       </c>
-      <c r="O5" s="5"/>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="N5">
+        <f t="shared" si="1"/>
+        <v>-262277.08999999985</v>
+      </c>
+      <c r="O5" s="5">
+        <f t="shared" si="2"/>
+        <v>-3.3800336357544182E-2</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1360,23 +2463,56 @@
       <c r="C6">
         <v>385908.52</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="D6">
+        <f>C6-B6</f>
+        <v>-23391.479999999981</v>
+      </c>
+      <c r="E6" s="5">
+        <f>IF(B6&lt;&gt;0, (C6-B6)/B6, IF(C6=0, 0, ""))</f>
+        <v>-5.7149963352064452E-2</v>
+      </c>
+      <c r="F6">
+        <f>IF(E6&lt;&gt;"", RANK(E6, $E$2:$E$52), "")</f>
+        <v>41</v>
+      </c>
       <c r="G6">
         <v>428500</v>
       </c>
       <c r="H6">
         <v>427758.64</v>
       </c>
-      <c r="J6" s="5"/>
+      <c r="I6">
+        <f>H6-G6</f>
+        <v>-741.35999999998603</v>
+      </c>
+      <c r="J6" s="5">
+        <f>IF(G6&lt;&gt;0, (H6-G6)/G6, IF(H6=0, 0, ""))</f>
+        <v>-1.7301283547257551E-3</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
       <c r="L6">
         <v>445200</v>
       </c>
       <c r="M6">
         <v>445114.28999999899</v>
       </c>
-      <c r="O6" s="5"/>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="N6">
+        <f t="shared" si="1"/>
+        <v>-85.710000001010485</v>
+      </c>
+      <c r="O6" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.925202156356929E-4</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1386,23 +2522,56 @@
       <c r="C7">
         <v>2946071.21</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="D7">
+        <f>C7-B7</f>
+        <v>-382928.79000000004</v>
+      </c>
+      <c r="E7" s="5">
+        <f>IF(B7&lt;&gt;0, (C7-B7)/B7, IF(C7=0, 0, ""))</f>
+        <v>-0.11502817362571344</v>
+      </c>
+      <c r="F7">
+        <f>IF(E7&lt;&gt;"", RANK(E7, $E$2:$E$52), "")</f>
+        <v>50</v>
+      </c>
       <c r="G7">
         <v>3390900</v>
       </c>
       <c r="H7">
         <v>3051483.41</v>
       </c>
-      <c r="J7" s="5"/>
+      <c r="I7">
+        <f>H7-G7</f>
+        <v>-339416.58999999985</v>
+      </c>
+      <c r="J7" s="5">
+        <f>IF(G7&lt;&gt;0, (H7-G7)/G7, IF(H7=0, 0, ""))</f>
+        <v>-0.10009631366303927</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
       <c r="L7">
         <v>3345200</v>
       </c>
       <c r="M7">
         <v>2946440.08</v>
       </c>
-      <c r="O7" s="5"/>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="N7">
+        <f t="shared" si="1"/>
+        <v>-398759.91999999993</v>
+      </c>
+      <c r="O7" s="5">
+        <f t="shared" si="2"/>
+        <v>-0.11920361114432618</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1412,23 +2581,56 @@
       <c r="C8">
         <v>1315623.30999999</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="D8">
+        <f>C8-B8</f>
+        <v>-236476.69000000996</v>
+      </c>
+      <c r="E8" s="5">
+        <f>IF(B8&lt;&gt;0, (C8-B8)/B8, IF(C8=0, 0, ""))</f>
+        <v>-0.15235918433091292</v>
+      </c>
+      <c r="F8">
+        <f>IF(E8&lt;&gt;"", RANK(E8, $E$2:$E$52), "")</f>
+        <v>51</v>
+      </c>
       <c r="G8">
         <v>1590700</v>
       </c>
       <c r="H8">
         <v>1383905.98999999</v>
       </c>
-      <c r="J8" s="5"/>
+      <c r="I8">
+        <f>H8-G8</f>
+        <v>-206794.01000001002</v>
+      </c>
+      <c r="J8" s="5">
+        <f>IF(G8&lt;&gt;0, (H8-G8)/G8, IF(H8=0, 0, ""))</f>
+        <v>-0.13000189224870184</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
       <c r="L8">
         <v>1579300</v>
       </c>
       <c r="M8">
         <v>1337735.3199999901</v>
       </c>
-      <c r="O8" s="5"/>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="N8">
+        <f t="shared" si="1"/>
+        <v>-241564.68000000995</v>
+      </c>
+      <c r="O8" s="5">
+        <f t="shared" si="2"/>
+        <v>-0.15295680364719175</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1438,23 +2640,56 @@
       <c r="C9">
         <v>8952825.2799999993</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="D9">
+        <f>C9-B9</f>
+        <v>-396574.72000000067</v>
+      </c>
+      <c r="E9" s="5">
+        <f>IF(B9&lt;&gt;0, (C9-B9)/B9, IF(C9=0, 0, ""))</f>
+        <v>-4.2417130511048909E-2</v>
+      </c>
+      <c r="F9">
+        <f>IF(E9&lt;&gt;"", RANK(E9, $E$2:$E$52), "")</f>
+        <v>36</v>
+      </c>
       <c r="G9">
         <v>11073700</v>
       </c>
       <c r="H9">
         <v>9929059.5199999996</v>
       </c>
-      <c r="J9" s="5"/>
+      <c r="I9">
+        <f>H9-G9</f>
+        <v>-1144640.4800000004</v>
+      </c>
+      <c r="J9" s="5">
+        <f>IF(G9&lt;&gt;0, (H9-G9)/G9, IF(H9=0, 0, ""))</f>
+        <v>-0.10336567542917005</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
       <c r="L9">
         <v>10790500</v>
       </c>
       <c r="M9">
         <v>9993599.52999999</v>
       </c>
-      <c r="O9" s="5"/>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="N9">
+        <f t="shared" si="1"/>
+        <v>-796900.47000000998</v>
+      </c>
+      <c r="O9" s="5">
+        <f t="shared" si="2"/>
+        <v>-7.3852043000788653E-2</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1464,23 +2699,56 @@
       <c r="C10">
         <v>407090.37</v>
       </c>
-      <c r="E10" s="5"/>
+      <c r="D10">
+        <f>C10-B10</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="E10" s="5">
+        <f>IF(B10&lt;&gt;0, (C10-B10)/B10, IF(C10=0, 0, ""))</f>
+        <v>-8.1681998646514792E-2</v>
+      </c>
+      <c r="F10">
+        <f>IF(E10&lt;&gt;"", RANK(E10, $E$2:$E$52), "")</f>
+        <v>46</v>
+      </c>
       <c r="G10">
         <v>495200</v>
       </c>
       <c r="H10">
         <v>467907.84000000003</v>
       </c>
-      <c r="J10" s="5"/>
+      <c r="I10">
+        <f>H10-G10</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="J10" s="5">
+        <f>IF(G10&lt;&gt;0, (H10-G10)/G10, IF(H10=0, 0, ""))</f>
+        <v>-5.5113408723747932E-2</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
       <c r="L10">
         <v>487500</v>
       </c>
       <c r="M10">
         <v>478318.92</v>
       </c>
-      <c r="O10" s="5"/>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="N10">
+        <f t="shared" si="1"/>
+        <v>-9181.0800000000163</v>
+      </c>
+      <c r="O10" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.883298461538465E-2</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1490,23 +2758,56 @@
       <c r="C11">
         <v>0</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="D11">
+        <f>C11-B11</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <f>IF(B11&lt;&gt;0, (C11-B11)/B11, IF(C11=0, 0, ""))</f>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f>IF(E11&lt;&gt;"", RANK(E11, $E$2:$E$52), "")</f>
+        <v>2</v>
+      </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
-      <c r="J11" s="5"/>
+      <c r="I11">
+        <f>H11-G11</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
+        <f>IF(G11&lt;&gt;0, (H11-G11)/G11, IF(H11=0, 0, ""))</f>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="L11">
         <v>375000</v>
       </c>
       <c r="M11">
         <v>63771.91</v>
       </c>
-      <c r="O11" s="5"/>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>-311228.08999999997</v>
+      </c>
+      <c r="O11" s="5">
+        <f t="shared" si="2"/>
+        <v>-0.82994157333333329</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1516,23 +2817,56 @@
       <c r="C12">
         <v>4066595.33</v>
       </c>
-      <c r="E12" s="5"/>
+      <c r="D12">
+        <f>C12-B12</f>
+        <v>-214304.66999999993</v>
+      </c>
+      <c r="E12" s="5">
+        <f>IF(B12&lt;&gt;0, (C12-B12)/B12, IF(C12=0, 0, ""))</f>
+        <v>-5.0060657805601608E-2</v>
+      </c>
+      <c r="F12">
+        <f>IF(E12&lt;&gt;"", RANK(E12, $E$2:$E$52), "")</f>
+        <v>39</v>
+      </c>
       <c r="G12">
         <v>4700400</v>
       </c>
       <c r="H12">
         <v>4205555.5999999996</v>
       </c>
-      <c r="J12" s="5"/>
+      <c r="I12">
+        <f>H12-G12</f>
+        <v>-494844.40000000037</v>
+      </c>
+      <c r="J12" s="5">
+        <f>IF(G12&lt;&gt;0, (H12-G12)/G12, IF(H12=0, 0, ""))</f>
+        <v>-0.10527708280146378</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
       <c r="L12">
         <v>4677800</v>
       </c>
       <c r="M12">
         <v>4371713.1399999997</v>
       </c>
-      <c r="O12" s="5"/>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="N12">
+        <f t="shared" si="1"/>
+        <v>-306086.86000000034</v>
+      </c>
+      <c r="O12" s="5">
+        <f t="shared" si="2"/>
+        <v>-6.5433934755654441E-2</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1542,23 +2876,56 @@
       <c r="C13">
         <v>5772288.3300000001</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="D13">
+        <f>C13-B13</f>
+        <v>-75511.669999999925</v>
+      </c>
+      <c r="E13" s="5">
+        <f>IF(B13&lt;&gt;0, (C13-B13)/B13, IF(C13=0, 0, ""))</f>
+        <v>-1.2912833886247806E-2</v>
+      </c>
+      <c r="F13">
+        <f>IF(E13&lt;&gt;"", RANK(E13, $E$2:$E$52), "")</f>
+        <v>19</v>
+      </c>
       <c r="G13">
         <v>6223700</v>
       </c>
       <c r="H13">
         <v>5909077.9399999902</v>
       </c>
-      <c r="J13" s="5"/>
+      <c r="I13">
+        <f>H13-G13</f>
+        <v>-314622.06000000983</v>
+      </c>
+      <c r="J13" s="5">
+        <f>IF(G13&lt;&gt;0, (H13-G13)/G13, IF(H13=0, 0, ""))</f>
+        <v>-5.0552253482656594E-2</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
       <c r="L13">
         <v>6207300</v>
       </c>
       <c r="M13">
         <v>6056976.6699999999</v>
       </c>
-      <c r="O13" s="5"/>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>-150323.33000000007</v>
+      </c>
+      <c r="O13" s="5">
+        <f t="shared" si="2"/>
+        <v>-2.4217184605222895E-2</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1568,23 +2935,56 @@
       <c r="C14">
         <v>505017.37</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="D14">
+        <f>C14-B14</f>
+        <v>-6982.6300000000047</v>
+      </c>
+      <c r="E14" s="5">
+        <f>IF(B14&lt;&gt;0, (C14-B14)/B14, IF(C14=0, 0, ""))</f>
+        <v>-1.3637949218750009E-2</v>
+      </c>
+      <c r="F14">
+        <f>IF(E14&lt;&gt;"", RANK(E14, $E$2:$E$52), "")</f>
+        <v>22</v>
+      </c>
       <c r="G14">
         <v>530500</v>
       </c>
       <c r="H14">
         <v>524402.98</v>
       </c>
-      <c r="J14" s="5"/>
+      <c r="I14">
+        <f>H14-G14</f>
+        <v>-6097.0200000000186</v>
+      </c>
+      <c r="J14" s="5">
+        <f>IF(G14&lt;&gt;0, (H14-G14)/G14, IF(H14=0, 0, ""))</f>
+        <v>-1.1492968897266765E-2</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
       <c r="L14">
         <v>526200</v>
       </c>
       <c r="M14">
         <v>504989.88</v>
       </c>
-      <c r="O14" s="5"/>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="N14">
+        <f t="shared" si="1"/>
+        <v>-21210.119999999995</v>
+      </c>
+      <c r="O14" s="5">
+        <f t="shared" si="2"/>
+        <v>-4.0308095781071827E-2</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1594,23 +2994,56 @@
       <c r="C15">
         <v>156545919.90000001</v>
       </c>
-      <c r="E15" s="5"/>
+      <c r="D15">
+        <f>C15-B15</f>
+        <v>496819.90000000596</v>
+      </c>
+      <c r="E15" s="5">
+        <f>IF(B15&lt;&gt;0, (C15-B15)/B15, IF(C15=0, 0, ""))</f>
+        <v>3.1837408866824991E-3</v>
+      </c>
+      <c r="F15">
+        <f>IF(E15&lt;&gt;"", RANK(E15, $E$2:$E$52), "")</f>
+        <v>1</v>
+      </c>
       <c r="G15">
         <v>184167800</v>
       </c>
       <c r="H15">
         <v>175966389.24999899</v>
       </c>
-      <c r="J15" s="5"/>
+      <c r="I15">
+        <f>H15-G15</f>
+        <v>-8201410.7500010133</v>
+      </c>
+      <c r="J15" s="5">
+        <f>IF(G15&lt;&gt;0, (H15-G15)/G15, IF(H15=0, 0, ""))</f>
+        <v>-4.4532273014072019E-2</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
       <c r="L15">
         <v>188953500</v>
       </c>
       <c r="M15">
         <v>184450910.84999901</v>
       </c>
-      <c r="O15" s="5"/>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>-4502589.1500009894</v>
+      </c>
+      <c r="O15" s="5">
+        <f t="shared" si="2"/>
+        <v>-2.3829085727446114E-2</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1620,23 +3053,56 @@
       <c r="C16">
         <v>6522480.4599999897</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="D16">
+        <f>C16-B16</f>
+        <v>-78219.540000010282</v>
+      </c>
+      <c r="E16" s="5">
+        <f>IF(B16&lt;&gt;0, (C16-B16)/B16, IF(C16=0, 0, ""))</f>
+        <v>-1.1850188616360429E-2</v>
+      </c>
+      <c r="F16">
+        <f>IF(E16&lt;&gt;"", RANK(E16, $E$2:$E$52), "")</f>
+        <v>15</v>
+      </c>
       <c r="G16">
         <v>7352500</v>
       </c>
       <c r="H16">
         <v>7350464.0800000001</v>
       </c>
-      <c r="J16" s="5"/>
+      <c r="I16">
+        <f>H16-G16</f>
+        <v>-2035.9199999999255</v>
+      </c>
+      <c r="J16" s="5">
+        <f>IF(G16&lt;&gt;0, (H16-G16)/G16, IF(H16=0, 0, ""))</f>
+        <v>-2.769017341040361E-4</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
       <c r="L16">
         <v>7397200</v>
       </c>
       <c r="M16">
         <v>7397093</v>
       </c>
-      <c r="O16" s="5"/>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="N16">
+        <f t="shared" si="1"/>
+        <v>-107</v>
+      </c>
+      <c r="O16" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.4464932677229222E-5</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1646,23 +3112,56 @@
       <c r="C17">
         <v>14439480.050000001</v>
       </c>
-      <c r="E17" s="5"/>
+      <c r="D17">
+        <f>C17-B17</f>
+        <v>-421319.94999999925</v>
+      </c>
+      <c r="E17" s="5">
+        <f>IF(B17&lt;&gt;0, (C17-B17)/B17, IF(C17=0, 0, ""))</f>
+        <v>-2.8351094826658003E-2</v>
+      </c>
+      <c r="F17">
+        <f>IF(E17&lt;&gt;"", RANK(E17, $E$2:$E$52), "")</f>
+        <v>31</v>
+      </c>
       <c r="G17">
         <v>15309700</v>
       </c>
       <c r="H17">
         <v>14645233.51</v>
       </c>
-      <c r="J17" s="5"/>
+      <c r="I17">
+        <f>H17-G17</f>
+        <v>-664466.49000000022</v>
+      </c>
+      <c r="J17" s="5">
+        <f>IF(G17&lt;&gt;0, (H17-G17)/G17, IF(H17=0, 0, ""))</f>
+        <v>-4.3401666263871937E-2</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
       <c r="L17">
         <v>15311800</v>
       </c>
       <c r="M17">
         <v>14346057.039999999</v>
       </c>
-      <c r="O17" s="5"/>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="N17">
+        <f t="shared" si="1"/>
+        <v>-965742.96000000089</v>
+      </c>
+      <c r="O17" s="5">
+        <f t="shared" si="2"/>
+        <v>-6.3071811282801551E-2</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1672,23 +3171,56 @@
       <c r="C18">
         <v>2615303.8999999901</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="D18">
+        <f>C18-B18</f>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="E18" s="5">
+        <f>IF(B18&lt;&gt;0, (C18-B18)/B18, IF(C18=0, 0, ""))</f>
+        <v>-5.4037002206391245E-2</v>
+      </c>
+      <c r="F18">
+        <f>IF(E18&lt;&gt;"", RANK(E18, $E$2:$E$52), "")</f>
+        <v>40</v>
+      </c>
       <c r="G18">
         <v>2861000</v>
       </c>
       <c r="H18">
         <v>2671745.94</v>
       </c>
-      <c r="J18" s="5"/>
+      <c r="I18">
+        <f>H18-G18</f>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="J18" s="5">
+        <f>IF(G18&lt;&gt;0, (H18-G18)/G18, IF(H18=0, 0, ""))</f>
+        <v>-6.6149619014330668E-2</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
       <c r="L18">
         <v>2910600</v>
       </c>
       <c r="M18">
         <v>2535637.09</v>
       </c>
-      <c r="O18" s="5"/>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="N18">
+        <f t="shared" si="1"/>
+        <v>-374962.91000000015</v>
+      </c>
+      <c r="O18" s="5">
+        <f t="shared" si="2"/>
+        <v>-0.12882667147667154</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1698,23 +3230,56 @@
       <c r="C19">
         <v>8460963.1999999899</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="D19">
+        <f>C19-B19</f>
+        <v>-376336.80000001006</v>
+      </c>
+      <c r="E19" s="5">
+        <f>IF(B19&lt;&gt;0, (C19-B19)/B19, IF(C19=0, 0, ""))</f>
+        <v>-4.258504294298146E-2</v>
+      </c>
+      <c r="F19">
+        <f>IF(E19&lt;&gt;"", RANK(E19, $E$2:$E$52), "")</f>
+        <v>37</v>
+      </c>
       <c r="G19">
         <v>9713300</v>
       </c>
       <c r="H19">
         <v>8991707.2399999909</v>
       </c>
-      <c r="J19" s="5"/>
+      <c r="I19">
+        <f>H19-G19</f>
+        <v>-721592.76000000909</v>
+      </c>
+      <c r="J19" s="5">
+        <f>IF(G19&lt;&gt;0, (H19-G19)/G19, IF(H19=0, 0, ""))</f>
+        <v>-7.4289145810384635E-2</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
       <c r="L19">
         <v>9343000</v>
       </c>
       <c r="M19">
         <v>8766655.9100000001</v>
       </c>
-      <c r="O19" s="5"/>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="N19">
+        <f t="shared" si="1"/>
+        <v>-576344.08999999985</v>
+      </c>
+      <c r="O19" s="5">
+        <f t="shared" si="2"/>
+        <v>-6.1687262121374278E-2</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1724,23 +3289,56 @@
       <c r="C20">
         <v>124384360.159999</v>
       </c>
-      <c r="E20" s="5"/>
+      <c r="D20">
+        <f>C20-B20</f>
+        <v>-1539.8400010019541</v>
+      </c>
+      <c r="E20" s="5">
+        <f>IF(B20&lt;&gt;0, (C20-B20)/B20, IF(C20=0, 0, ""))</f>
+        <v>-1.2379538203300809E-5</v>
+      </c>
+      <c r="F20">
+        <f>IF(E20&lt;&gt;"", RANK(E20, $E$2:$E$52), "")</f>
+        <v>6</v>
+      </c>
       <c r="G20">
         <v>131849400</v>
       </c>
       <c r="H20">
         <v>131839624.37</v>
       </c>
-      <c r="J20" s="5"/>
+      <c r="I20">
+        <f>H20-G20</f>
+        <v>-9775.6299999952316</v>
+      </c>
+      <c r="J20" s="5">
+        <f>IF(G20&lt;&gt;0, (H20-G20)/G20, IF(H20=0, 0, ""))</f>
+        <v>-7.4142392760188761E-5</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="L20">
         <v>130621400</v>
       </c>
       <c r="M20">
         <v>130621283.53999899</v>
       </c>
-      <c r="O20" s="5"/>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="N20">
+        <f t="shared" si="1"/>
+        <v>-116.46000100672245</v>
+      </c>
+      <c r="O20" s="5">
+        <f t="shared" si="2"/>
+        <v>-8.9158438821450736E-7</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -1750,23 +3348,56 @@
       <c r="C21">
         <v>22408587.5499999</v>
       </c>
-      <c r="E21" s="5"/>
+      <c r="D21">
+        <f>C21-B21</f>
+        <v>-1923512.4500000998</v>
+      </c>
+      <c r="E21" s="5">
+        <f>IF(B21&lt;&gt;0, (C21-B21)/B21, IF(C21=0, 0, ""))</f>
+        <v>-7.9052463618023094E-2</v>
+      </c>
+      <c r="F21">
+        <f>IF(E21&lt;&gt;"", RANK(E21, $E$2:$E$52), "")</f>
+        <v>43</v>
+      </c>
       <c r="G21">
         <v>24497400</v>
       </c>
       <c r="H21">
         <v>22655993.629999999</v>
       </c>
-      <c r="J21" s="5"/>
+      <c r="I21">
+        <f>H21-G21</f>
+        <v>-1841406.370000001</v>
+      </c>
+      <c r="J21" s="5">
+        <f>IF(G21&lt;&gt;0, (H21-G21)/G21, IF(H21=0, 0, ""))</f>
+        <v>-7.5167420624229556E-2</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
       <c r="L21">
         <v>24323000</v>
       </c>
       <c r="M21">
         <v>23434073.089999899</v>
       </c>
-      <c r="O21" s="5"/>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="N21">
+        <f t="shared" si="1"/>
+        <v>-888926.91000010073</v>
+      </c>
+      <c r="O21" s="5">
+        <f t="shared" si="2"/>
+        <v>-3.6546762734864152E-2</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1776,23 +3407,56 @@
       <c r="C22">
         <v>11412339.8799999</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="D22">
+        <f>C22-B22</f>
+        <v>-153660.12000009976</v>
+      </c>
+      <c r="E22" s="5">
+        <f>IF(B22&lt;&gt;0, (C22-B22)/B22, IF(C22=0, 0, ""))</f>
+        <v>-1.3285502334437123E-2</v>
+      </c>
+      <c r="F22">
+        <f>IF(E22&lt;&gt;"", RANK(E22, $E$2:$E$52), "")</f>
+        <v>20</v>
+      </c>
       <c r="G22">
         <v>11980700</v>
       </c>
       <c r="H22">
         <v>11791977.9699999</v>
       </c>
-      <c r="J22" s="5"/>
+      <c r="I22">
+        <f>H22-G22</f>
+        <v>-188722.03000009991</v>
+      </c>
+      <c r="J22" s="5">
+        <f>IF(G22&lt;&gt;0, (H22-G22)/G22, IF(H22=0, 0, ""))</f>
+        <v>-1.5752170574348738E-2</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
       <c r="L22">
         <v>11935200</v>
       </c>
       <c r="M22">
         <v>11934454.77</v>
       </c>
-      <c r="O22" s="5"/>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="N22">
+        <f t="shared" si="1"/>
+        <v>-745.23000000044703</v>
+      </c>
+      <c r="O22" s="5">
+        <f t="shared" si="2"/>
+        <v>-6.2439674240938325E-5</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -1802,23 +3466,56 @@
       <c r="C23">
         <v>20036743.4099999</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="D23">
+        <f>C23-B23</f>
+        <v>-825956.59000010043</v>
+      </c>
+      <c r="E23" s="5">
+        <f>IF(B23&lt;&gt;0, (C23-B23)/B23, IF(C23=0, 0, ""))</f>
+        <v>-3.9590110100806722E-2</v>
+      </c>
+      <c r="F23">
+        <f>IF(E23&lt;&gt;"", RANK(E23, $E$2:$E$52), "")</f>
+        <v>34</v>
+      </c>
       <c r="G23">
         <v>22683800</v>
       </c>
       <c r="H23">
         <v>21722126.219999898</v>
       </c>
-      <c r="J23" s="5"/>
+      <c r="I23">
+        <f>H23-G23</f>
+        <v>-961673.78000010177</v>
+      </c>
+      <c r="J23" s="5">
+        <f>IF(G23&lt;&gt;0, (H23-G23)/G23, IF(H23=0, 0, ""))</f>
+        <v>-4.2394738976719144E-2</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
       <c r="L23">
         <v>23220300</v>
       </c>
       <c r="M23">
         <v>22619057.440000001</v>
       </c>
-      <c r="O23" s="5"/>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="N23">
+        <f t="shared" si="1"/>
+        <v>-601242.55999999866</v>
+      </c>
+      <c r="O23" s="5">
+        <f t="shared" si="2"/>
+        <v>-2.5892971236375011E-2</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1828,23 +3525,56 @@
       <c r="C24">
         <v>904969.19</v>
       </c>
-      <c r="E24" s="5"/>
+      <c r="D24">
+        <f>C24-B24</f>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="E24" s="5">
+        <f>IF(B24&lt;&gt;0, (C24-B24)/B24, IF(C24=0, 0, ""))</f>
+        <v>-1.3334943305713101E-2</v>
+      </c>
+      <c r="F24">
+        <f>IF(E24&lt;&gt;"", RANK(E24, $E$2:$E$52), "")</f>
+        <v>21</v>
+      </c>
       <c r="G24">
         <v>1112700</v>
       </c>
       <c r="H24">
         <v>1067214.42</v>
       </c>
-      <c r="J24" s="5"/>
+      <c r="I24">
+        <f>H24-G24</f>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="J24" s="5">
+        <f>IF(G24&lt;&gt;0, (H24-G24)/G24, IF(H24=0, 0, ""))</f>
+        <v>-4.087856565111897E-2</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
       <c r="L24">
         <v>1112600</v>
       </c>
       <c r="M24">
         <v>1112527.1200000001</v>
       </c>
-      <c r="O24" s="5"/>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="N24">
+        <f t="shared" si="1"/>
+        <v>-72.879999999888241</v>
+      </c>
+      <c r="O24" s="5">
+        <f t="shared" si="2"/>
+        <v>-6.5504224339284781E-5</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1854,23 +3584,56 @@
       <c r="C25">
         <v>479149.53</v>
       </c>
-      <c r="E25" s="5"/>
+      <c r="D25">
+        <f>C25-B25</f>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="E25" s="5">
+        <f>IF(B25&lt;&gt;0, (C25-B25)/B25, IF(C25=0, 0, ""))</f>
+        <v>-1.0226130964676661E-2</v>
+      </c>
+      <c r="F25">
+        <f>IF(E25&lt;&gt;"", RANK(E25, $E$2:$E$52), "")</f>
+        <v>14</v>
+      </c>
       <c r="G25">
         <v>505200</v>
       </c>
       <c r="H25">
         <v>497194.20999999897</v>
       </c>
-      <c r="J25" s="5"/>
+      <c r="I25">
+        <f>H25-G25</f>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="J25" s="5">
+        <f>IF(G25&lt;&gt;0, (H25-G25)/G25, IF(H25=0, 0, ""))</f>
+        <v>-1.5846773555029746E-2</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
       <c r="L25">
         <v>496500</v>
       </c>
       <c r="M25">
         <v>494775.1</v>
       </c>
-      <c r="O25" s="5"/>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="N25">
+        <f t="shared" si="1"/>
+        <v>-1724.9000000000233</v>
+      </c>
+      <c r="O25" s="5">
+        <f t="shared" si="2"/>
+        <v>-3.4741188318228064E-3</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -1880,23 +3643,56 @@
       <c r="C26">
         <v>4801960.08</v>
       </c>
-      <c r="E26" s="5"/>
+      <c r="D26">
+        <f>C26-B26</f>
+        <v>-447839.91999999993</v>
+      </c>
+      <c r="E26" s="5">
+        <f>IF(B26&lt;&gt;0, (C26-B26)/B26, IF(C26=0, 0, ""))</f>
+        <v>-8.5306091660634673E-2</v>
+      </c>
+      <c r="F26">
+        <f>IF(E26&lt;&gt;"", RANK(E26, $E$2:$E$52), "")</f>
+        <v>47</v>
+      </c>
       <c r="G26">
         <v>5442200</v>
       </c>
       <c r="H26">
         <v>5122329.02999999</v>
       </c>
-      <c r="J26" s="5"/>
+      <c r="I26">
+        <f>H26-G26</f>
+        <v>-319870.97000000998</v>
+      </c>
+      <c r="J26" s="5">
+        <f>IF(G26&lt;&gt;0, (H26-G26)/G26, IF(H26=0, 0, ""))</f>
+        <v>-5.8776040939327839E-2</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
       <c r="L26">
         <v>5430700</v>
       </c>
       <c r="M26">
         <v>5117235.21</v>
       </c>
-      <c r="O26" s="5"/>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="N26">
+        <f t="shared" si="1"/>
+        <v>-313464.79000000004</v>
+      </c>
+      <c r="O26" s="5">
+        <f t="shared" si="2"/>
+        <v>-5.7720881286022069E-2</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -1906,23 +3702,56 @@
       <c r="C27">
         <v>0</v>
       </c>
-      <c r="E27" s="5"/>
+      <c r="D27">
+        <f>C27-B27</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="5">
+        <f>IF(B27&lt;&gt;0, (C27-B27)/B27, IF(C27=0, 0, ""))</f>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f>IF(E27&lt;&gt;"", RANK(E27, $E$2:$E$52), "")</f>
+        <v>2</v>
+      </c>
       <c r="G27">
         <v>0</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
-      <c r="J27" s="5"/>
+      <c r="I27">
+        <f>H27-G27</f>
+        <v>0</v>
+      </c>
+      <c r="J27" s="5">
+        <f>IF(G27&lt;&gt;0, (H27-G27)/G27, IF(H27=0, 0, ""))</f>
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="L27">
         <v>0</v>
       </c>
       <c r="M27">
         <v>0</v>
       </c>
-      <c r="O27" s="5"/>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="N27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O27" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1932,23 +3761,56 @@
       <c r="C28">
         <v>1250442.02</v>
       </c>
-      <c r="E28" s="5"/>
+      <c r="D28">
+        <f>C28-B28</f>
+        <v>-132457.97999999998</v>
+      </c>
+      <c r="E28" s="5">
+        <f>IF(B28&lt;&gt;0, (C28-B28)/B28, IF(C28=0, 0, ""))</f>
+        <v>-9.5782760864849215E-2</v>
+      </c>
+      <c r="F28">
+        <f>IF(E28&lt;&gt;"", RANK(E28, $E$2:$E$52), "")</f>
+        <v>49</v>
+      </c>
       <c r="G28">
         <v>1545700</v>
       </c>
       <c r="H28">
         <v>1281335.23</v>
       </c>
-      <c r="J28" s="5"/>
+      <c r="I28">
+        <f>H28-G28</f>
+        <v>-264364.77</v>
+      </c>
+      <c r="J28" s="5">
+        <f>IF(G28&lt;&gt;0, (H28-G28)/G28, IF(H28=0, 0, ""))</f>
+        <v>-0.17103239309050916</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
       <c r="L28">
         <v>1525900</v>
       </c>
       <c r="M28">
         <v>1393285.06</v>
       </c>
-      <c r="O28" s="5"/>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="N28">
+        <f t="shared" si="1"/>
+        <v>-132614.93999999994</v>
+      </c>
+      <c r="O28" s="5">
+        <f t="shared" si="2"/>
+        <v>-8.6909325643882263E-2</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -1958,23 +3820,56 @@
       <c r="C29">
         <v>2523884.71</v>
       </c>
-      <c r="E29" s="5"/>
+      <c r="D29">
+        <f>C29-B29</f>
+        <v>-37915.290000000037</v>
+      </c>
+      <c r="E29" s="5">
+        <f>IF(B29&lt;&gt;0, (C29-B29)/B29, IF(C29=0, 0, ""))</f>
+        <v>-1.4800253727847622E-2</v>
+      </c>
+      <c r="F29">
+        <f>IF(E29&lt;&gt;"", RANK(E29, $E$2:$E$52), "")</f>
+        <v>24</v>
+      </c>
       <c r="G29">
         <v>2779500</v>
       </c>
       <c r="H29">
         <v>2665264.4399999902</v>
       </c>
-      <c r="J29" s="5"/>
+      <c r="I29">
+        <f>H29-G29</f>
+        <v>-114235.56000000983</v>
+      </c>
+      <c r="J29" s="5">
+        <f>IF(G29&lt;&gt;0, (H29-G29)/G29, IF(H29=0, 0, ""))</f>
+        <v>-4.1099320021590155E-2</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
       <c r="L29">
         <v>2889900</v>
       </c>
       <c r="M29">
         <v>2889864.67</v>
       </c>
-      <c r="O29" s="5"/>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="N29">
+        <f t="shared" si="1"/>
+        <v>-35.330000000074506</v>
+      </c>
+      <c r="O29" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.2225336516860273E-5</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -1984,23 +3879,56 @@
       <c r="C30">
         <v>12030494.1</v>
       </c>
-      <c r="E30" s="5"/>
+      <c r="D30">
+        <f>C30-B30</f>
+        <v>-101705.90000000037</v>
+      </c>
+      <c r="E30" s="5">
+        <f>IF(B30&lt;&gt;0, (C30-B30)/B30, IF(C30=0, 0, ""))</f>
+        <v>-8.3831374359143746E-3</v>
+      </c>
+      <c r="F30">
+        <f>IF(E30&lt;&gt;"", RANK(E30, $E$2:$E$52), "")</f>
+        <v>12</v>
+      </c>
       <c r="G30">
         <v>12735900</v>
       </c>
       <c r="H30">
         <v>12685514.279999901</v>
       </c>
-      <c r="J30" s="5"/>
+      <c r="I30">
+        <f>H30-G30</f>
+        <v>-50385.720000099391</v>
+      </c>
+      <c r="J30" s="5">
+        <f>IF(G30&lt;&gt;0, (H30-G30)/G30, IF(H30=0, 0, ""))</f>
+        <v>-3.9561962641116366E-3</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="L30">
         <v>12861300</v>
       </c>
       <c r="M30">
         <v>12826009.609999999</v>
       </c>
-      <c r="O30" s="5"/>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="N30">
+        <f t="shared" si="1"/>
+        <v>-35290.390000000596</v>
+      </c>
+      <c r="O30" s="5">
+        <f t="shared" si="2"/>
+        <v>-2.7439209100169185E-3</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -2010,23 +3938,56 @@
       <c r="C31">
         <v>1740827.69</v>
       </c>
-      <c r="E31" s="5"/>
+      <c r="D31">
+        <f>C31-B31</f>
+        <v>-24772.310000000056</v>
+      </c>
+      <c r="E31" s="5">
+        <f>IF(B31&lt;&gt;0, (C31-B31)/B31, IF(C31=0, 0, ""))</f>
+        <v>-1.4030533529678329E-2</v>
+      </c>
+      <c r="F31">
+        <f>IF(E31&lt;&gt;"", RANK(E31, $E$2:$E$52), "")</f>
+        <v>23</v>
+      </c>
       <c r="G31">
         <v>1823300</v>
       </c>
       <c r="H31">
         <v>1762676.85</v>
       </c>
-      <c r="J31" s="5"/>
+      <c r="I31">
+        <f>H31-G31</f>
+        <v>-60623.149999999907</v>
+      </c>
+      <c r="J31" s="5">
+        <f>IF(G31&lt;&gt;0, (H31-G31)/G31, IF(H31=0, 0, ""))</f>
+        <v>-3.3249136181648611E-2</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
       <c r="L31">
         <v>1870700</v>
       </c>
       <c r="M31">
         <v>1801391.34</v>
       </c>
-      <c r="O31" s="5"/>
-    </row>
-    <row r="32" spans="1:15">
+      <c r="N31">
+        <f t="shared" si="1"/>
+        <v>-69308.659999999916</v>
+      </c>
+      <c r="O31" s="5">
+        <f t="shared" si="2"/>
+        <v>-3.7049585716576634E-2</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -2036,23 +3997,56 @@
       <c r="C32">
         <v>5925637.7199999904</v>
       </c>
-      <c r="E32" s="5"/>
+      <c r="D32">
+        <f>C32-B32</f>
+        <v>-73762.280000009574</v>
+      </c>
+      <c r="E32" s="5">
+        <f>IF(B32&lt;&gt;0, (C32-B32)/B32, IF(C32=0, 0, ""))</f>
+        <v>-1.2294942827617691E-2</v>
+      </c>
+      <c r="F32">
+        <f>IF(E32&lt;&gt;"", RANK(E32, $E$2:$E$52), "")</f>
+        <v>16</v>
+      </c>
       <c r="G32">
         <v>6195500</v>
       </c>
       <c r="H32">
         <v>6084985.4699999997</v>
       </c>
-      <c r="J32" s="5"/>
+      <c r="I32">
+        <f>H32-G32</f>
+        <v>-110514.53000000026</v>
+      </c>
+      <c r="J32" s="5">
+        <f>IF(G32&lt;&gt;0, (H32-G32)/G32, IF(H32=0, 0, ""))</f>
+        <v>-1.7837871035428981E-2</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
       <c r="L32">
         <v>6157400</v>
       </c>
       <c r="M32">
         <v>5987572.0199999996</v>
       </c>
-      <c r="O32" s="5"/>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="N32">
+        <f t="shared" si="1"/>
+        <v>-169827.98000000045</v>
+      </c>
+      <c r="O32" s="5">
+        <f t="shared" si="2"/>
+        <v>-2.7581118653977402E-2</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -2062,23 +4056,56 @@
       <c r="C33">
         <v>920284264.73000002</v>
       </c>
-      <c r="E33" s="5"/>
+      <c r="D33">
+        <f>C33-B33</f>
+        <v>-7418835.2699990273</v>
+      </c>
+      <c r="E33" s="5">
+        <f>IF(B33&lt;&gt;0, (C33-B33)/B33, IF(C33=0, 0, ""))</f>
+        <v>-7.9969930789269058E-3</v>
+      </c>
+      <c r="F33">
+        <f>IF(E33&lt;&gt;"", RANK(E33, $E$2:$E$52), "")</f>
+        <v>11</v>
+      </c>
       <c r="G33">
         <v>979671000</v>
       </c>
       <c r="H33">
         <v>977068513.48000002</v>
       </c>
-      <c r="J33" s="5"/>
+      <c r="I33">
+        <f>H33-G33</f>
+        <v>-2602486.5199999809</v>
+      </c>
+      <c r="J33" s="5">
+        <f>IF(G33&lt;&gt;0, (H33-G33)/G33, IF(H33=0, 0, ""))</f>
+        <v>-2.6564903115433454E-3</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
       <c r="L33">
         <v>989572899.99999905</v>
       </c>
       <c r="M33">
         <v>984116289.40999901</v>
       </c>
-      <c r="O33" s="5"/>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="N33">
+        <f t="shared" si="1"/>
+        <v>-5456610.5900000334</v>
+      </c>
+      <c r="O33" s="5">
+        <f t="shared" si="2"/>
+        <v>-5.5141067323084929E-3</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -2088,23 +4115,56 @@
       <c r="C34">
         <v>4109958.22</v>
       </c>
-      <c r="E34" s="5"/>
+      <c r="D34">
+        <f>C34-B34</f>
+        <v>-79341.779999999795</v>
+      </c>
+      <c r="E34" s="5">
+        <f>IF(B34&lt;&gt;0, (C34-B34)/B34, IF(C34=0, 0, ""))</f>
+        <v>-1.8939149738619768E-2</v>
+      </c>
+      <c r="F34">
+        <f>IF(E34&lt;&gt;"", RANK(E34, $E$2:$E$52), "")</f>
+        <v>26</v>
+      </c>
       <c r="G34">
         <v>4350600</v>
       </c>
       <c r="H34">
         <v>4137588.7699999898</v>
       </c>
-      <c r="J34" s="5"/>
+      <c r="I34">
+        <f>H34-G34</f>
+        <v>-213011.23000001023</v>
+      </c>
+      <c r="J34" s="5">
+        <f>IF(G34&lt;&gt;0, (H34-G34)/G34, IF(H34=0, 0, ""))</f>
+        <v>-4.8961345561534093E-2</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
       <c r="L34">
         <v>4345600</v>
       </c>
       <c r="M34">
         <v>4229801.51</v>
       </c>
-      <c r="O34" s="5"/>
-    </row>
-    <row r="35" spans="1:15">
+      <c r="N34">
+        <f t="shared" si="1"/>
+        <v>-115798.49000000022</v>
+      </c>
+      <c r="O34" s="5">
+        <f t="shared" si="2"/>
+        <v>-2.6647296115611244E-2</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -2114,23 +4174,56 @@
       <c r="C35">
         <v>0</v>
       </c>
-      <c r="E35" s="5"/>
+      <c r="D35">
+        <f>C35-B35</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="5">
+        <f>IF(B35&lt;&gt;0, (C35-B35)/B35, IF(C35=0, 0, ""))</f>
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <f>IF(E35&lt;&gt;"", RANK(E35, $E$2:$E$52), "")</f>
+        <v>2</v>
+      </c>
       <c r="G35">
         <v>0</v>
       </c>
       <c r="H35">
         <v>0</v>
       </c>
-      <c r="J35" s="5"/>
+      <c r="I35">
+        <f>H35-G35</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="5">
+        <f>IF(G35&lt;&gt;0, (H35-G35)/G35, IF(H35=0, 0, ""))</f>
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="L35">
         <v>0</v>
       </c>
       <c r="M35">
         <v>0</v>
       </c>
-      <c r="O35" s="5"/>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="N35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O35" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -2140,23 +4233,56 @@
       <c r="C36">
         <v>735423.27999999898</v>
       </c>
-      <c r="E36" s="5"/>
+      <c r="D36">
+        <f>C36-B36</f>
+        <v>-62776.72000000102</v>
+      </c>
+      <c r="E36" s="5">
+        <f>IF(B36&lt;&gt;0, (C36-B36)/B36, IF(C36=0, 0, ""))</f>
+        <v>-7.8647857679780775E-2</v>
+      </c>
+      <c r="F36">
+        <f>IF(E36&lt;&gt;"", RANK(E36, $E$2:$E$52), "")</f>
+        <v>42</v>
+      </c>
       <c r="G36">
         <v>898700</v>
       </c>
       <c r="H36">
         <v>740966.94999999902</v>
       </c>
-      <c r="J36" s="5"/>
+      <c r="I36">
+        <f>H36-G36</f>
+        <v>-157733.05000000098</v>
+      </c>
+      <c r="J36" s="5">
+        <f>IF(G36&lt;&gt;0, (H36-G36)/G36, IF(H36=0, 0, ""))</f>
+        <v>-0.17551246244575608</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
       <c r="L36">
         <v>878300</v>
       </c>
       <c r="M36">
         <v>777215.28999999899</v>
       </c>
-      <c r="O36" s="5"/>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="N36">
+        <f t="shared" si="1"/>
+        <v>-101084.71000000101</v>
+      </c>
+      <c r="O36" s="5">
+        <f t="shared" si="2"/>
+        <v>-0.11509132414892521</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -2166,23 +4292,56 @@
       <c r="C37">
         <v>2005447.73999999</v>
       </c>
-      <c r="E37" s="5"/>
+      <c r="D37">
+        <f>C37-B37</f>
+        <v>-82352.260000010021</v>
+      </c>
+      <c r="E37" s="5">
+        <f>IF(B37&lt;&gt;0, (C37-B37)/B37, IF(C37=0, 0, ""))</f>
+        <v>-3.9444515758219188E-2</v>
+      </c>
+      <c r="F37">
+        <f>IF(E37&lt;&gt;"", RANK(E37, $E$2:$E$52), "")</f>
+        <v>33</v>
+      </c>
       <c r="G37">
         <v>2229200</v>
       </c>
       <c r="H37">
         <v>2118943.21</v>
       </c>
-      <c r="J37" s="5"/>
+      <c r="I37">
+        <f>H37-G37</f>
+        <v>-110256.79000000004</v>
+      </c>
+      <c r="J37" s="5">
+        <f>IF(G37&lt;&gt;0, (H37-G37)/G37, IF(H37=0, 0, ""))</f>
+        <v>-4.9460250314014013E-2</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
       <c r="L37">
         <v>2296900</v>
       </c>
       <c r="M37">
         <v>2108718.34</v>
       </c>
-      <c r="O37" s="5"/>
-    </row>
-    <row r="38" spans="1:15">
+      <c r="N37">
+        <f t="shared" si="1"/>
+        <v>-188181.66000000015</v>
+      </c>
+      <c r="O37" s="5">
+        <f t="shared" si="2"/>
+        <v>-8.1928538464887526E-2</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -2192,23 +4351,56 @@
       <c r="C38">
         <v>838669.82</v>
       </c>
-      <c r="E38" s="5"/>
+      <c r="D38">
+        <f>C38-B38</f>
+        <v>-16630.180000000051</v>
+      </c>
+      <c r="E38" s="5">
+        <f>IF(B38&lt;&gt;0, (C38-B38)/B38, IF(C38=0, 0, ""))</f>
+        <v>-1.9443680579913542E-2</v>
+      </c>
+      <c r="F38">
+        <f>IF(E38&lt;&gt;"", RANK(E38, $E$2:$E$52), "")</f>
+        <v>27</v>
+      </c>
       <c r="G38">
         <v>792800</v>
       </c>
       <c r="H38">
         <v>753451.96</v>
       </c>
-      <c r="J38" s="5"/>
+      <c r="I38">
+        <f>H38-G38</f>
+        <v>-39348.040000000037</v>
+      </c>
+      <c r="J38" s="5">
+        <f>IF(G38&lt;&gt;0, (H38-G38)/G38, IF(H38=0, 0, ""))</f>
+        <v>-4.9631735620585316E-2</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
       <c r="L38">
         <v>777800</v>
       </c>
       <c r="M38">
         <v>777663.26</v>
       </c>
-      <c r="O38" s="5"/>
-    </row>
-    <row r="39" spans="1:15">
+      <c r="N38">
+        <f t="shared" si="1"/>
+        <v>-136.73999999999069</v>
+      </c>
+      <c r="O38" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.7580354847003174E-4</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>53</v>
       </c>
@@ -2218,23 +4410,56 @@
       <c r="C39">
         <v>813108.87</v>
       </c>
-      <c r="E39" s="5"/>
+      <c r="D39">
+        <f>C39-B39</f>
+        <v>-70791.13</v>
+      </c>
+      <c r="E39" s="5">
+        <f>IF(B39&lt;&gt;0, (C39-B39)/B39, IF(C39=0, 0, ""))</f>
+        <v>-8.008952370177623E-2</v>
+      </c>
+      <c r="F39">
+        <f>IF(E39&lt;&gt;"", RANK(E39, $E$2:$E$52), "")</f>
+        <v>44</v>
+      </c>
       <c r="G39">
         <v>1294400</v>
       </c>
       <c r="H39">
         <v>1114242.27999999</v>
       </c>
-      <c r="J39" s="5"/>
+      <c r="I39">
+        <f>H39-G39</f>
+        <v>-180157.72000000998</v>
+      </c>
+      <c r="J39" s="5">
+        <f>IF(G39&lt;&gt;0, (H39-G39)/G39, IF(H39=0, 0, ""))</f>
+        <v>-0.13918241656366656</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
       <c r="L39">
         <v>1759500</v>
       </c>
       <c r="M39">
         <v>1680463.8699999901</v>
       </c>
-      <c r="O39" s="5"/>
-    </row>
-    <row r="40" spans="1:15">
+      <c r="N39">
+        <f t="shared" si="1"/>
+        <v>-79036.1300000099</v>
+      </c>
+      <c r="O39" s="5">
+        <f t="shared" si="2"/>
+        <v>-4.4919653310605226E-2</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -2244,23 +4469,56 @@
       <c r="C40">
         <v>37565141.859999903</v>
       </c>
-      <c r="E40" s="5"/>
+      <c r="D40">
+        <f>C40-B40</f>
+        <v>-816758.14000009745</v>
+      </c>
+      <c r="E40" s="5">
+        <f>IF(B40&lt;&gt;0, (C40-B40)/B40, IF(C40=0, 0, ""))</f>
+        <v>-2.1279773539092578E-2</v>
+      </c>
+      <c r="F40">
+        <f>IF(E40&lt;&gt;"", RANK(E40, $E$2:$E$52), "")</f>
+        <v>29</v>
+      </c>
       <c r="G40">
         <v>39964900</v>
       </c>
       <c r="H40">
         <v>38095240.189999901</v>
       </c>
-      <c r="J40" s="5"/>
+      <c r="I40">
+        <f>H40-G40</f>
+        <v>-1869659.8100000992</v>
+      </c>
+      <c r="J40" s="5">
+        <f>IF(G40&lt;&gt;0, (H40-G40)/G40, IF(H40=0, 0, ""))</f>
+        <v>-4.6782546934937892E-2</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
       <c r="L40">
         <v>40216700</v>
       </c>
       <c r="M40">
         <v>39606263.709999897</v>
       </c>
-      <c r="O40" s="5"/>
-    </row>
-    <row r="41" spans="1:15">
+      <c r="N40">
+        <f t="shared" si="1"/>
+        <v>-610436.29000010341</v>
+      </c>
+      <c r="O40" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.5178676768608648E-2</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -2270,23 +4528,56 @@
       <c r="C41">
         <v>4409060.2099999897</v>
       </c>
-      <c r="E41" s="5"/>
+      <c r="D41">
+        <f>C41-B41</f>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="E41" s="5">
+        <f>IF(B41&lt;&gt;0, (C41-B41)/B41, IF(C41=0, 0, ""))</f>
+        <v>-4.0110550149132493E-2</v>
+      </c>
+      <c r="F41">
+        <f>IF(E41&lt;&gt;"", RANK(E41, $E$2:$E$52), "")</f>
+        <v>35</v>
+      </c>
       <c r="G41">
         <v>5089500</v>
       </c>
       <c r="H41">
         <v>4956043.6699999897</v>
       </c>
-      <c r="J41" s="5"/>
+      <c r="I41">
+        <f>H41-G41</f>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="J41" s="5">
+        <f>IF(G41&lt;&gt;0, (H41-G41)/G41, IF(H41=0, 0, ""))</f>
+        <v>-2.6221894095689226E-2</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
       <c r="L41">
         <v>4799900</v>
       </c>
       <c r="M41">
         <v>4717822.6500000004</v>
       </c>
-      <c r="O41" s="5"/>
-    </row>
-    <row r="42" spans="1:15">
+      <c r="N41">
+        <f t="shared" si="1"/>
+        <v>-82077.349999999627</v>
+      </c>
+      <c r="O41" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.7099804162586642E-2</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -2296,23 +4587,56 @@
       <c r="C42">
         <v>188551675.67999899</v>
       </c>
-      <c r="E42" s="5"/>
+      <c r="D42">
+        <f>C42-B42</f>
+        <v>-41624.320001006126</v>
+      </c>
+      <c r="E42" s="5">
+        <f>IF(B42&lt;&gt;0, (C42-B42)/B42, IF(C42=0, 0, ""))</f>
+        <v>-2.2070943135841053E-4</v>
+      </c>
+      <c r="F42">
+        <f>IF(E42&lt;&gt;"", RANK(E42, $E$2:$E$52), "")</f>
+        <v>8</v>
+      </c>
       <c r="G42">
         <v>199130300</v>
       </c>
       <c r="H42">
         <v>196755033.31</v>
       </c>
-      <c r="J42" s="5"/>
+      <c r="I42">
+        <f>H42-G42</f>
+        <v>-2375266.6899999976</v>
+      </c>
+      <c r="J42" s="5">
+        <f>IF(G42&lt;&gt;0, (H42-G42)/G42, IF(H42=0, 0, ""))</f>
+        <v>-1.1928203241796942E-2</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
       <c r="L42">
         <v>199954600</v>
       </c>
       <c r="M42">
         <v>199954563.74999899</v>
       </c>
-      <c r="O42" s="5"/>
-    </row>
-    <row r="43" spans="1:15">
+      <c r="N42">
+        <f t="shared" si="1"/>
+        <v>-36.250001013278961</v>
+      </c>
+      <c r="O42" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.8129115815929696E-7</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>57</v>
       </c>
@@ -2322,23 +4646,56 @@
       <c r="C43">
         <v>7968645.8300000001</v>
       </c>
-      <c r="E43" s="5"/>
+      <c r="D43">
+        <f>C43-B43</f>
+        <v>-166754.16999999993</v>
+      </c>
+      <c r="E43" s="5">
+        <f>IF(B43&lt;&gt;0, (C43-B43)/B43, IF(C43=0, 0, ""))</f>
+        <v>-2.0497353541313264E-2</v>
+      </c>
+      <c r="F43">
+        <f>IF(E43&lt;&gt;"", RANK(E43, $E$2:$E$52), "")</f>
+        <v>28</v>
+      </c>
       <c r="G43">
         <v>8560800</v>
       </c>
       <c r="H43">
         <v>8171472.0199999996</v>
       </c>
-      <c r="J43" s="5"/>
+      <c r="I43">
+        <f>H43-G43</f>
+        <v>-389327.98000000045</v>
+      </c>
+      <c r="J43" s="5">
+        <f>IF(G43&lt;&gt;0, (H43-G43)/G43, IF(H43=0, 0, ""))</f>
+        <v>-4.5477990374731388E-2</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
       <c r="L43">
         <v>8497500</v>
       </c>
       <c r="M43">
         <v>8150982.5699999901</v>
       </c>
-      <c r="O43" s="5"/>
-    </row>
-    <row r="44" spans="1:15">
+      <c r="N43">
+        <f t="shared" si="1"/>
+        <v>-346517.43000000995</v>
+      </c>
+      <c r="O43" s="5">
+        <f t="shared" si="2"/>
+        <v>-4.0778750220654303E-2</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -2348,23 +4705,56 @@
       <c r="C44">
         <v>29789104.379999999</v>
       </c>
-      <c r="E44" s="5"/>
+      <c r="D44">
+        <f>C44-B44</f>
+        <v>-294095.62000000104</v>
+      </c>
+      <c r="E44" s="5">
+        <f>IF(B44&lt;&gt;0, (C44-B44)/B44, IF(C44=0, 0, ""))</f>
+        <v>-9.7760750186150751E-3</v>
+      </c>
+      <c r="F44">
+        <f>IF(E44&lt;&gt;"", RANK(E44, $E$2:$E$52), "")</f>
+        <v>13</v>
+      </c>
       <c r="G44">
         <v>31040700</v>
       </c>
       <c r="H44">
         <v>30793711.48</v>
       </c>
-      <c r="J44" s="5"/>
+      <c r="I44">
+        <f>H44-G44</f>
+        <v>-246988.51999999955</v>
+      </c>
+      <c r="J44" s="5">
+        <f>IF(G44&lt;&gt;0, (H44-G44)/G44, IF(H44=0, 0, ""))</f>
+        <v>-7.9569249404813532E-3</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
       <c r="L44">
         <v>31282200</v>
       </c>
       <c r="M44">
         <v>31282141.25</v>
       </c>
-      <c r="O44" s="5"/>
-    </row>
-    <row r="45" spans="1:15">
+      <c r="N44">
+        <f t="shared" si="1"/>
+        <v>-58.75</v>
+      </c>
+      <c r="O44" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.8780648419868168E-6</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>59</v>
       </c>
@@ -2374,23 +4764,56 @@
       <c r="C45">
         <v>54589584.0499999</v>
       </c>
-      <c r="E45" s="5"/>
+      <c r="D45">
+        <f>C45-B45</f>
+        <v>-712015.95000009984</v>
+      </c>
+      <c r="E45" s="5">
+        <f>IF(B45&lt;&gt;0, (C45-B45)/B45, IF(C45=0, 0, ""))</f>
+        <v>-1.287514194887851E-2</v>
+      </c>
+      <c r="F45">
+        <f>IF(E45&lt;&gt;"", RANK(E45, $E$2:$E$52), "")</f>
+        <v>18</v>
+      </c>
       <c r="G45">
         <v>56792200</v>
       </c>
       <c r="H45">
         <v>54594953.959999897</v>
       </c>
-      <c r="J45" s="5"/>
+      <c r="I45">
+        <f>H45-G45</f>
+        <v>-2197246.0400001034</v>
+      </c>
+      <c r="J45" s="5">
+        <f>IF(G45&lt;&gt;0, (H45-G45)/G45, IF(H45=0, 0, ""))</f>
+        <v>-3.8689222111488959E-2</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
       <c r="L45">
         <v>56027100</v>
       </c>
       <c r="M45">
         <v>55386549.6599999</v>
       </c>
-      <c r="O45" s="5"/>
-    </row>
-    <row r="46" spans="1:15">
+      <c r="N45">
+        <f t="shared" si="1"/>
+        <v>-640550.34000010043</v>
+      </c>
+      <c r="O45" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.1432866237947358E-2</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>60</v>
       </c>
@@ -2400,23 +4823,56 @@
       <c r="C46">
         <v>258322.43</v>
       </c>
-      <c r="E46" s="5"/>
+      <c r="D46">
+        <f>C46-B46</f>
+        <v>-777.57000000000698</v>
+      </c>
+      <c r="E46" s="5">
+        <f>IF(B46&lt;&gt;0, (C46-B46)/B46, IF(C46=0, 0, ""))</f>
+        <v>-3.0010420686993711E-3</v>
+      </c>
+      <c r="F46">
+        <f>IF(E46&lt;&gt;"", RANK(E46, $E$2:$E$52), "")</f>
+        <v>9</v>
+      </c>
       <c r="G46">
         <v>266000</v>
       </c>
       <c r="H46">
         <v>257402.90999999901</v>
       </c>
-      <c r="J46" s="5"/>
+      <c r="I46">
+        <f>H46-G46</f>
+        <v>-8597.090000000986</v>
+      </c>
+      <c r="J46" s="5">
+        <f>IF(G46&lt;&gt;0, (H46-G46)/G46, IF(H46=0, 0, ""))</f>
+        <v>-3.2319887218048821E-2</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
       <c r="L46">
         <v>267100</v>
       </c>
       <c r="M46">
         <v>254753.15999999901</v>
       </c>
-      <c r="O46" s="5"/>
-    </row>
-    <row r="47" spans="1:15">
+      <c r="N46">
+        <f t="shared" si="1"/>
+        <v>-12346.840000000986</v>
+      </c>
+      <c r="O46" s="5">
+        <f t="shared" si="2"/>
+        <v>-4.6225533508053113E-2</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>61</v>
       </c>
@@ -2426,23 +4882,56 @@
       <c r="C47">
         <v>70378426.719999999</v>
       </c>
-      <c r="E47" s="5"/>
+      <c r="D47">
+        <f>C47-B47</f>
+        <v>-12273.280000001192</v>
+      </c>
+      <c r="E47" s="5">
+        <f>IF(B47&lt;&gt;0, (C47-B47)/B47, IF(C47=0, 0, ""))</f>
+        <v>-1.7435939690898361E-4</v>
+      </c>
+      <c r="F47">
+        <f>IF(E47&lt;&gt;"", RANK(E47, $E$2:$E$52), "")</f>
+        <v>7</v>
+      </c>
       <c r="G47">
         <v>73467000</v>
       </c>
       <c r="H47">
         <v>73442541.659999996</v>
       </c>
-      <c r="J47" s="5"/>
+      <c r="I47">
+        <f>H47-G47</f>
+        <v>-24458.340000003576</v>
+      </c>
+      <c r="J47" s="5">
+        <f>IF(G47&lt;&gt;0, (H47-G47)/G47, IF(H47=0, 0, ""))</f>
+        <v>-3.3291600310348285E-4</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
       <c r="L47">
         <v>75072800</v>
       </c>
       <c r="M47">
         <v>75050829.179999903</v>
       </c>
-      <c r="O47" s="5"/>
-    </row>
-    <row r="48" spans="1:15">
+      <c r="N47">
+        <f t="shared" si="1"/>
+        <v>-21970.820000097156</v>
+      </c>
+      <c r="O47" s="5">
+        <f t="shared" si="2"/>
+        <v>-2.9266019117572752E-4</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>62</v>
       </c>
@@ -2452,23 +4941,56 @@
       <c r="C48">
         <v>6527352.5699999901</v>
       </c>
-      <c r="E48" s="5"/>
+      <c r="D48">
+        <f>C48-B48</f>
+        <v>-209747.43000000995</v>
+      </c>
+      <c r="E48" s="5">
+        <f>IF(B48&lt;&gt;0, (C48-B48)/B48, IF(C48=0, 0, ""))</f>
+        <v>-3.1133192323107857E-2</v>
+      </c>
+      <c r="F48">
+        <f>IF(E48&lt;&gt;"", RANK(E48, $E$2:$E$52), "")</f>
+        <v>32</v>
+      </c>
       <c r="G48">
         <v>7214700</v>
       </c>
       <c r="H48">
         <v>6922072.5599999996</v>
       </c>
-      <c r="J48" s="5"/>
+      <c r="I48">
+        <f>H48-G48</f>
+        <v>-292627.44000000041</v>
+      </c>
+      <c r="J48" s="5">
+        <f>IF(G48&lt;&gt;0, (H48-G48)/G48, IF(H48=0, 0, ""))</f>
+        <v>-4.0559890224125802E-2</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
       <c r="L48">
         <v>7289800</v>
       </c>
       <c r="M48">
         <v>6882350.23999999</v>
       </c>
-      <c r="O48" s="5"/>
-    </row>
-    <row r="49" spans="1:15">
+      <c r="N48">
+        <f t="shared" si="1"/>
+        <v>-407449.76000001002</v>
+      </c>
+      <c r="O48" s="5">
+        <f t="shared" si="2"/>
+        <v>-5.5893132870587676E-2</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -2478,23 +5000,56 @@
       <c r="C49">
         <v>90499.43</v>
       </c>
-      <c r="E49" s="5"/>
+      <c r="D49">
+        <f>C49-B49</f>
+        <v>-1700.570000000007</v>
+      </c>
+      <c r="E49" s="5">
+        <f>IF(B49&lt;&gt;0, (C49-B49)/B49, IF(C49=0, 0, ""))</f>
+        <v>-1.8444360086767971E-2</v>
+      </c>
+      <c r="F49">
+        <f>IF(E49&lt;&gt;"", RANK(E49, $E$2:$E$52), "")</f>
+        <v>25</v>
+      </c>
       <c r="G49">
         <v>102600</v>
       </c>
       <c r="H49">
         <v>95466.880000000005</v>
       </c>
-      <c r="J49" s="5"/>
+      <c r="I49">
+        <f>H49-G49</f>
+        <v>-7133.1199999999953</v>
+      </c>
+      <c r="J49" s="5">
+        <f>IF(G49&lt;&gt;0, (H49-G49)/G49, IF(H49=0, 0, ""))</f>
+        <v>-6.9523586744639335E-2</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
       <c r="L49">
         <v>0</v>
       </c>
       <c r="M49">
         <v>0</v>
       </c>
-      <c r="O49" s="5"/>
-    </row>
-    <row r="50" spans="1:15">
+      <c r="N49">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O49" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -2504,23 +5059,56 @@
       <c r="C50">
         <v>832600</v>
       </c>
-      <c r="E50" s="5"/>
+      <c r="D50">
+        <f>C50-B50</f>
+        <v>0</v>
+      </c>
+      <c r="E50" s="5">
+        <f>IF(B50&lt;&gt;0, (C50-B50)/B50, IF(C50=0, 0, ""))</f>
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <f>IF(E50&lt;&gt;"", RANK(E50, $E$2:$E$52), "")</f>
+        <v>2</v>
+      </c>
       <c r="G50">
         <v>859100</v>
       </c>
       <c r="H50">
         <v>859100</v>
       </c>
-      <c r="J50" s="5"/>
+      <c r="I50">
+        <f>H50-G50</f>
+        <v>0</v>
+      </c>
+      <c r="J50" s="5">
+        <f>IF(G50&lt;&gt;0, (H50-G50)/G50, IF(H50=0, 0, ""))</f>
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="L50">
         <v>843200</v>
       </c>
       <c r="M50">
         <v>843200</v>
       </c>
-      <c r="O50" s="5"/>
-    </row>
-    <row r="51" spans="1:15">
+      <c r="N50">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O50" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>65</v>
       </c>
@@ -2530,23 +5118,56 @@
       <c r="C51">
         <v>8499425.3399999905</v>
       </c>
-      <c r="E51" s="5"/>
+      <c r="D51">
+        <f>C51-B51</f>
+        <v>-110074.66000000946</v>
+      </c>
+      <c r="E51" s="5">
+        <f>IF(B51&lt;&gt;0, (C51-B51)/B51, IF(C51=0, 0, ""))</f>
+        <v>-1.2785255822058129E-2</v>
+      </c>
+      <c r="F51">
+        <f>IF(E51&lt;&gt;"", RANK(E51, $E$2:$E$52), "")</f>
+        <v>17</v>
+      </c>
       <c r="G51">
         <v>8925500</v>
       </c>
       <c r="H51">
         <v>8599059.6199999992</v>
       </c>
-      <c r="J51" s="5"/>
+      <c r="I51">
+        <f>H51-G51</f>
+        <v>-326440.38000000082</v>
+      </c>
+      <c r="J51" s="5">
+        <f>IF(G51&lt;&gt;0, (H51-G51)/G51, IF(H51=0, 0, ""))</f>
+        <v>-3.6573903982970231E-2</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
       <c r="L51">
         <v>8833900</v>
       </c>
       <c r="M51">
         <v>8735843.3100000005</v>
       </c>
-      <c r="O51" s="5"/>
-    </row>
-    <row r="52" spans="1:15">
+      <c r="N51">
+        <f t="shared" si="1"/>
+        <v>-98056.689999999478</v>
+      </c>
+      <c r="O51" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.1100045280114048E-2</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>66</v>
       </c>
@@ -2556,28 +5177,61 @@
       <c r="C52">
         <v>2254684.7999999998</v>
       </c>
-      <c r="E52" s="5"/>
+      <c r="D52">
+        <f>C52-B52</f>
+        <v>-196315.20000000019</v>
+      </c>
+      <c r="E52" s="5">
+        <f>IF(B52&lt;&gt;0, (C52-B52)/B52, IF(C52=0, 0, ""))</f>
+        <v>-8.009596083231342E-2</v>
+      </c>
+      <c r="F52">
+        <f>IF(E52&lt;&gt;"", RANK(E52, $E$2:$E$52), "")</f>
+        <v>45</v>
+      </c>
       <c r="G52">
         <v>2440700</v>
       </c>
       <c r="H52">
         <v>2204672.88</v>
       </c>
-      <c r="J52" s="5"/>
+      <c r="I52">
+        <f>H52-G52</f>
+        <v>-236027.12000000011</v>
+      </c>
+      <c r="J52" s="5">
+        <f>IF(G52&lt;&gt;0, (H52-G52)/G52, IF(H52=0, 0, ""))</f>
+        <v>-9.6704683082722218E-2</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
       <c r="L52">
         <v>2321600</v>
       </c>
       <c r="M52">
         <v>2056835.26</v>
       </c>
-      <c r="O52" s="5"/>
-    </row>
-    <row r="54" spans="1:15" ht="15">
+      <c r="N52">
+        <f t="shared" si="1"/>
+        <v>-264764.74</v>
+      </c>
+      <c r="O52" s="5">
+        <f t="shared" si="2"/>
+        <v>-0.11404408166781529</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -2591,42 +5245,114 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="57" spans="1:15">
+      <c r="B56">
+        <f>INDEX($D$1:$N$52, MATCH($A56, $A$1:$A$52, 0), MATCH(B$55, $D$1:$N$1, 0))</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="C56">
+        <f>INDEX($D$1:$N$52, MATCH($A56, $A$1:$A$52, 0), MATCH(C$55, $D$1:$N$1, 0))</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="D56">
+        <f t="shared" ref="C56:D61" si="4">INDEX($D$1:$N$52, MATCH($A56, $A$1:$A$52, 0), MATCH(D$55, $D$1:$N$1, 0))</f>
+        <v>-9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="58" spans="1:15">
+      <c r="B57">
+        <f t="shared" ref="B57:B61" si="5">INDEX($D$1:$N$52, MATCH($A57, $A$1:$A$52, 0), MATCH(B$55, $D$1:$N$1, 0))</f>
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="4"/>
+        <v>-311228.08999999997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="59" spans="1:15">
+      <c r="B58">
+        <f t="shared" si="5"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="4"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="4"/>
+        <v>-374962.91000000015</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="60" spans="1:15">
+      <c r="B59">
+        <f t="shared" si="5"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="4"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="4"/>
+        <v>-72.879999999888241</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="61" spans="1:15">
+      <c r="B60">
+        <f t="shared" si="5"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="4"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="4"/>
+        <v>-1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" ht="15">
+      <c r="B61">
+        <f t="shared" si="5"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="4"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="4"/>
+        <v>-82077.349999999627</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
@@ -2640,43 +5366,114 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="15">
+      <c r="B65">
+        <f>_xlfn.XLOOKUP(A65,$A$1:$A$52,$D$1:$D$52)</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="C65">
+        <f>_xlfn.XLOOKUP(A65,$A$1:$A$52,$I$1:$I$52)</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="D65">
+        <f>_xlfn.XLOOKUP(A65,$A$1:$A$52,$N$1:$N$52)</f>
+        <v>-9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" ht="15">
+      <c r="B66">
+        <f t="shared" ref="B66:B70" si="6">_xlfn.XLOOKUP(A66,$A$1:$A$52,$D$1:$D$52)</f>
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <f t="shared" ref="C66:C70" si="7">_xlfn.XLOOKUP(A66,$A$1:$A$52,$I$1:$I$52)</f>
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <f t="shared" ref="D66:D70" si="8">_xlfn.XLOOKUP(A66,$A$1:$A$52,$N$1:$N$52)</f>
+        <v>-311228.08999999997</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="B67">
+        <f t="shared" si="6"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="7"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="8"/>
+        <v>-374962.91000000015</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="B68">
+        <f t="shared" si="6"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="7"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="8"/>
+        <v>-72.879999999888241</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="B69">
+        <f t="shared" si="6"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="7"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="8"/>
+        <v>-1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="15"/>
-    <row r="72" spans="1:4" ht="15">
+      <c r="B70">
+        <f>_xlfn.XLOOKUP(A70,$A$1:$A$52,$D$1:$D$52)</f>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="7"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="8"/>
+        <v>-82077.349999999627</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -2690,48 +5487,119 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" ht="15">
+      <c r="B74">
+        <f>INDEX($D$1:$D$52,MATCH(A74,$A$1:$A$52,0))</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="C74">
+        <f>INDEX($I$1:$I$52,MATCH(A74,$A$1:$A$52,0))</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="D74">
+        <f>INDEX($N$1:$N$52,MATCH(A74,$A$1:$A$52,0))</f>
+        <v>-9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
+      <c r="B75">
+        <f t="shared" ref="B75:B79" si="9">INDEX($D$1:$D$52,MATCH(A75,$A$1:$A$52,0))</f>
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <f t="shared" ref="C75:C79" si="10">INDEX($I$1:$I$52,MATCH(A75,$A$1:$A$52,0))</f>
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <f t="shared" ref="D75:D79" si="11">INDEX($N$1:$N$52,MATCH(A75,$A$1:$A$52,0))</f>
+        <v>-311228.08999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="B76">
+        <f t="shared" si="9"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="10"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="11"/>
+        <v>-374962.91000000015</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="B77">
+        <f t="shared" si="9"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="10"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="11"/>
+        <v>-72.879999999888241</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="79" spans="1:4">
+      <c r="B78">
+        <f t="shared" si="9"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="10"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="11"/>
+        <v>-1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="15"/>
-    <row r="81" spans="1:7" ht="15">
+      <c r="B79">
+        <f t="shared" si="9"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="10"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="11"/>
+        <v>-82077.349999999627</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
         <v>71</v>
       </c>
@@ -2739,34 +5607,56 @@
         <v>72</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>73</v>
       </c>
-      <c r="B84" s="6"/>
-      <c r="C84" s="6"/>
-    </row>
-    <row r="85" spans="1:7">
+      <c r="B84" s="6">
+        <f>INDEX($B$1:$C$52, MATCH(B87, $A$1:$A$52, 0), 1)</f>
+        <v>14860800</v>
+      </c>
+      <c r="C84" s="6">
+        <f>INDEX($B$1:$C$52, MATCH(B87, $A$1:$A$52, 0), 2)</f>
+        <v>14439480.050000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>74</v>
       </c>
-      <c r="B85" s="6"/>
-      <c r="C85" s="6"/>
-    </row>
-    <row r="86" spans="1:7">
+      <c r="B85" s="6">
+        <f>INDEX($G$1:$H$52, MATCH(B87, $A$1:$A$52, 0), 1)</f>
+        <v>15309700</v>
+      </c>
+      <c r="C85" s="6">
+        <f>INDEX($G$1:$H$52, MATCH(B87, $A$1:$A$52, 0), 2)</f>
+        <v>14645233.51</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="6"/>
-      <c r="C86" s="6"/>
-    </row>
-    <row r="87" spans="1:7" ht="15"/>
-    <row r="88" spans="1:7" ht="15">
+      <c r="B86" s="6">
+        <f>INDEX($L$1:$M$52, MATCH(B87, $A$1:$A$52, 0), 1)</f>
+        <v>15311800</v>
+      </c>
+      <c r="C86" s="6">
+        <f>INDEX($L$1:$M$52, MATCH(B87, $A$1:$A$52, 0), 2)</f>
+        <v>14346057.039999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>77</v>
       </c>
@@ -2782,7 +5672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="15">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B90" s="8" t="s">
         <v>0</v>
       </c>
@@ -2802,36 +5692,72 @@
         <v>78</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>73</v>
       </c>
+      <c r="B91" t="str">
+        <f>IFERROR(INDEX($A$2:$A$52, MATCH(1, $F$2:$F$52, 0)), "")</f>
+        <v>Debt Service</v>
+      </c>
       <c r="C91" s="5"/>
+      <c r="D91" t="str">
+        <f>IFERROR(INDEX($A$2:$A$52, MATCH(2, $F$2:$F$52, 0)), "")</f>
+        <v>Community Oversight Board</v>
+      </c>
       <c r="E91" s="5"/>
+      <c r="F91" t="str">
+        <f>IFERROR(INDEX($A$2:$A$52, MATCH(3, $F$2:$F$52, 0)), "")</f>
+        <v/>
+      </c>
       <c r="G91" s="5"/>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>74</v>
       </c>
+      <c r="B92" t="str">
+        <f>IFERROR(INDEX($A$2:$A$52, MATCH(1, $K$2:$K$52, 0)), "")</f>
+        <v>Community Oversight Board</v>
+      </c>
       <c r="C92" s="5"/>
+      <c r="D92" t="str">
+        <f>IFERROR(INDEX($A$2:$A$52, MATCH(2, $K$2:$K$52, 0)), "")</f>
+        <v/>
+      </c>
       <c r="E92" s="5"/>
+      <c r="F92" t="str">
+        <f>IFERROR(INDEX($A$2:$A$52, MATCH(3, $K$2:$K$52, 0)), "")</f>
+        <v/>
+      </c>
       <c r="G92" s="5"/>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>75</v>
       </c>
+      <c r="B93" t="str">
+        <f>IFERROR(INDEX($A$2:$A$52, MATCH(1, $P$2:$P$52, 0)), "")</f>
+        <v>Information Technology Service</v>
+      </c>
       <c r="C93" s="5"/>
+      <c r="D93" t="str">
+        <f>IFERROR(INDEX($A$2:$A$52, MATCH(1, $P$2:$P$52, 0)), "")</f>
+        <v>Information Technology Service</v>
+      </c>
       <c r="E93" s="5"/>
+      <c r="F93" t="str">
+        <f>IFERROR(INDEX($A$2:$A$52, MATCH(3, $P$2:$P$52, 0)), "")</f>
+        <v/>
+      </c>
       <c r="G93" s="5"/>
     </row>
-    <row r="95" spans="1:7" ht="15">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>77</v>
       </c>
@@ -2847,7 +5773,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="15">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B97" s="8" t="s">
         <v>0</v>
       </c>
@@ -2867,7 +5793,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>73</v>
       </c>
@@ -2876,7 +5802,7 @@
       <c r="G98" s="4"/>
       <c r="I98" s="4"/>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>74</v>
       </c>
@@ -2885,7 +5811,7 @@
       <c r="G99" s="4"/>
       <c r="I99" s="4"/>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>75</v>
       </c>
@@ -2894,20 +5820,18 @@
       <c r="G100" s="4"/>
       <c r="I100" s="4"/>
     </row>
-    <row r="102" spans="1:9" ht="15"/>
-    <row r="103" spans="1:9" ht="15"/>
-    <row r="104" spans="1:9" ht="15"/>
-    <row r="105" spans="1:9" ht="15"/>
-    <row r="106" spans="1:9" ht="15"/>
-    <row r="107" spans="1:9" ht="15"/>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
-      <formula1>$A$2:$A$52</formula1>
+  <dataValidations disablePrompts="1" count="3">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B87" xr:uid="{8FD59168-DBA6-4B68-A4C7-3F08B77EA969}">
+      <formula1>$A$1:$A$52</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B87" xr:uid="{2AD69E73-434A-4C8E-81A1-C486ADC07835}">
+      <formula1>$A$1:$A$51</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2919,13 +5843,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2933,7 +5857,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2941,7 +5865,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2949,7 +5873,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -2957,7 +5881,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -2965,7 +5889,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -2973,7 +5897,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -2981,7 +5905,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -2989,7 +5913,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -2997,7 +5921,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Changing some things from the revision.
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athelize\Desktop\NSS Data Analytics\Excel\lookups_exercise-Athelize\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3C65F0-436B-4547-815E-FE4B0F0CF545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FFF0CF-FF50-4A7C-95BE-79717A3B61AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -335,12 +335,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.000%"/>
-    <numFmt numFmtId="167" formatCode="0.0000%"/>
-    <numFmt numFmtId="168" formatCode="0.00000%"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -793,7 +790,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -836,9 +833,8 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -850,12 +846,8 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -895,7 +887,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -920,10 +911,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="103"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="3"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -934,7 +925,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>ECC Emergency Comm Center</c:v>
+              <c:v>Administrative</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -972,7 +963,7 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="bar"/>
+        <c:barDir val="col"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -994,7 +985,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent1">
+                <a:shade val="76000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1026,13 +1019,13 @@
                 <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>14860800</c:v>
+                  <c:v>356640100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15309700</c:v>
+                  <c:v>382685200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15311800</c:v>
+                  <c:v>376548600</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
                   <c:v>0</c:v>
@@ -1065,7 +1058,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent1">
+                <a:tint val="77000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1097,13 +1092,13 @@
                 <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>14439480.050000001</c:v>
+                  <c:v>341243679.13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14645233.51</c:v>
+                  <c:v>346340810.81999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14346057.039999999</c:v>
+                  <c:v>355279492.22999901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1132,9 +1127,9 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1183,9 +1178,9 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:numFmt formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1296,42 +1291,8 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
   <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -1850,8 +1811,8 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>819149</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>85</xdr:row>
       <xdr:rowOff>166687</xdr:rowOff>
     </xdr:to>
@@ -2180,8 +2141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2262,13 +2223,13 @@
         <f t="shared" ref="D2:D33" si="0">C2-B2</f>
         <v>-15396420.870000005</v>
       </c>
-      <c r="E2" s="10">
-        <f t="shared" ref="E2:E33" si="1">IF(B2&lt;&gt;0, (C2-B2)/B2, IF(C2=0, 0, ""))</f>
+      <c r="E2" s="5">
+        <f>IF(B2&lt;&gt;0, (C2-B2)/B2, IF(C2=0, 0,))</f>
         <v>-4.3170750765267295E-2</v>
       </c>
-      <c r="F2">
-        <f t="shared" ref="F2:F33" si="2">IF(E2&lt;&gt;"", RANK(E2, $E$2:$E$52), "")</f>
-        <v>38</v>
+      <c r="F2" t="e">
+        <f>IF(E2&lt;&gt;0, RANK(E11, $E$2:$E$52))</f>
+        <v>#VALUE!</v>
       </c>
       <c r="G2">
         <v>382685200</v>
@@ -2277,16 +2238,16 @@
         <v>346340810.81999999</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I33" si="3">H2-G2</f>
+        <f t="shared" ref="I2:I33" si="1">H2-G2</f>
         <v>-36344389.180000007</v>
       </c>
       <c r="J2" s="5">
-        <f t="shared" ref="J2:J33" si="4">IF(G2&lt;&gt;0, (H2-G2)/G2, IF(H2=0, 0, ""))</f>
+        <f>IF(G2&lt;&gt;0, (H2-G2)/G2, IF(H2=0, 0, ))</f>
         <v>-9.4972027086493035E-2</v>
       </c>
       <c r="K2">
-        <f>IF(J2&lt;&gt;"", RANK(J2, $J$2:$J$52, 0), "")</f>
-        <v>42</v>
+        <f>IF(J2&lt;&gt;0, RANK(J11, $J$2:$J$52))</f>
+        <v>1</v>
       </c>
       <c r="L2">
         <v>376548600</v>
@@ -2298,13 +2259,13 @@
         <f>M2-L2</f>
         <v>-21269107.770000994</v>
       </c>
-      <c r="O2" s="11">
-        <f>IF(L2&lt;&gt;0, (M2-L2)/L2, IF(M2=0, 0, ""))</f>
+      <c r="O2" s="5">
+        <f>IF(L2&lt;&gt;0, (M2-L2)/L2, IF(M2=0, 0))</f>
         <v>-5.6484362894991494E-2</v>
       </c>
       <c r="P2">
-        <f>IF(O2&lt;&gt;"", RANK(O2, $O$2:$O$52), "")</f>
-        <v>38</v>
+        <f>IF(O2&lt;&gt;0, RANK(O11, $O$2:$O$52))</f>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -2321,13 +2282,13 @@
         <f t="shared" si="0"/>
         <v>-7585.4099999999744</v>
       </c>
-      <c r="E3" s="10">
-        <f t="shared" si="1"/>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E52" si="2">IF(B3&lt;&gt;0, (C3-B3)/B3, IF(C3=0, 0,))</f>
         <v>-2.3069981751824741E-2</v>
       </c>
       <c r="F3">
-        <f t="shared" si="2"/>
-        <v>30</v>
+        <f t="shared" ref="F3:F10" si="3">IF(E3&lt;&gt;0, RANK(E12, $E$2:$E$52))</f>
+        <v>36</v>
       </c>
       <c r="G3">
         <v>334800</v>
@@ -2336,16 +2297,16 @@
         <v>312433.70999999897</v>
       </c>
       <c r="I3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-22366.290000001027</v>
       </c>
       <c r="J3" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="J3:J52" si="4">IF(G3&lt;&gt;0, (H3-G3)/G3, IF(H3=0, 0, ))</f>
         <v>-6.6804928315415249E-2</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K52" si="5">IF(J3&lt;&gt;"", RANK(J3, $J$2:$J$52, 0), "")</f>
-        <v>38</v>
+        <f t="shared" ref="K3:K52" si="5">IF(J3&lt;&gt;0, RANK(J12, $J$2:$J$52))</f>
+        <v>46</v>
       </c>
       <c r="L3">
         <v>322700</v>
@@ -2357,13 +2318,13 @@
         <f t="shared" ref="N3:N52" si="6">M3-L3</f>
         <v>-436.96000000002095</v>
       </c>
-      <c r="O3" s="11">
-        <f t="shared" ref="O3:O52" si="7">IF(L3&lt;&gt;0, (M3-L3)/L3, IF(M3=0, 0, ""))</f>
+      <c r="O3" s="5">
+        <f t="shared" ref="O3:O52" si="7">IF(L3&lt;&gt;0, (M3-L3)/L3, IF(M3=0, 0))</f>
         <v>-1.3540749922529313E-3</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P52" si="8">IF(O3&lt;&gt;"", RANK(O3, $O$2:$O$52), "")</f>
-        <v>15</v>
+        <f t="shared" ref="P3:P52" si="8">IF(O3&lt;&gt;0, RANK(O12, $O$2:$O$52))</f>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -2380,13 +2341,13 @@
         <f t="shared" si="0"/>
         <v>-15442.440000010189</v>
       </c>
-      <c r="E4" s="10">
-        <f t="shared" si="1"/>
+      <c r="E4" s="5">
+        <f t="shared" si="2"/>
         <v>-4.9327413275443007E-3</v>
       </c>
       <c r="F4">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>16</v>
       </c>
       <c r="G4">
         <v>3652300</v>
@@ -2395,7 +2356,7 @@
         <v>3589693.2099999902</v>
       </c>
       <c r="I4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-62606.790000009816</v>
       </c>
       <c r="J4" s="5">
@@ -2404,7 +2365,7 @@
       </c>
       <c r="K4">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="L4">
         <v>3662400</v>
@@ -2416,13 +2377,13 @@
         <f t="shared" si="6"/>
         <v>-97416.950000009965</v>
       </c>
-      <c r="O4" s="11">
+      <c r="O4" s="5">
         <f t="shared" si="7"/>
         <v>-2.6599210899959033E-2</v>
       </c>
       <c r="P4">
         <f t="shared" si="8"/>
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -2439,13 +2400,13 @@
         <f t="shared" si="0"/>
         <v>-723147.33000000007</v>
       </c>
-      <c r="E5" s="10">
-        <f t="shared" si="1"/>
+      <c r="E5" s="5">
+        <f t="shared" si="2"/>
         <v>-9.4273968477453174E-2</v>
       </c>
       <c r="F5">
-        <f t="shared" si="2"/>
-        <v>48</v>
+        <f t="shared" si="3"/>
+        <v>19</v>
       </c>
       <c r="G5">
         <v>7968300</v>
@@ -2454,7 +2415,7 @@
         <v>7020609.3200000003</v>
       </c>
       <c r="I5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-947690.6799999997</v>
       </c>
       <c r="J5" s="5">
@@ -2463,7 +2424,7 @@
       </c>
       <c r="K5">
         <f t="shared" si="5"/>
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="L5">
         <v>7759600</v>
@@ -2475,13 +2436,13 @@
         <f t="shared" si="6"/>
         <v>-262277.08999999985</v>
       </c>
-      <c r="O5" s="11">
+      <c r="O5" s="5">
         <f t="shared" si="7"/>
         <v>-3.3800336357544182E-2</v>
       </c>
       <c r="P5">
         <f t="shared" si="8"/>
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -2498,13 +2459,13 @@
         <f t="shared" si="0"/>
         <v>-23391.479999999981</v>
       </c>
-      <c r="E6" s="10">
-        <f t="shared" si="1"/>
+      <c r="E6" s="5">
+        <f t="shared" si="2"/>
         <v>-5.7149963352064452E-2</v>
       </c>
       <c r="F6">
-        <f t="shared" si="2"/>
-        <v>41</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="G6">
         <v>428500</v>
@@ -2513,7 +2474,7 @@
         <v>427758.64</v>
       </c>
       <c r="I6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-741.35999999998603</v>
       </c>
       <c r="J6" s="5">
@@ -2522,7 +2483,7 @@
       </c>
       <c r="K6">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="L6">
         <v>445200</v>
@@ -2534,13 +2495,13 @@
         <f t="shared" si="6"/>
         <v>-85.710000001010485</v>
       </c>
-      <c r="O6" s="11">
+      <c r="O6" s="5">
         <f t="shared" si="7"/>
         <v>-1.925202156356929E-4</v>
       </c>
       <c r="P6">
         <f t="shared" si="8"/>
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -2557,13 +2518,13 @@
         <f t="shared" si="0"/>
         <v>-382928.79000000004</v>
       </c>
-      <c r="E7" s="10">
-        <f t="shared" si="1"/>
+      <c r="E7" s="5">
+        <f t="shared" si="2"/>
         <v>-0.11502817362571344</v>
       </c>
       <c r="F7">
-        <f t="shared" si="2"/>
-        <v>50</v>
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
       <c r="G7">
         <v>3390900</v>
@@ -2572,7 +2533,7 @@
         <v>3051483.41</v>
       </c>
       <c r="I7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-339416.58999999985</v>
       </c>
       <c r="J7" s="5">
@@ -2581,7 +2542,7 @@
       </c>
       <c r="K7">
         <f t="shared" si="5"/>
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="L7">
         <v>3345200</v>
@@ -2593,13 +2554,13 @@
         <f t="shared" si="6"/>
         <v>-398759.91999999993</v>
       </c>
-      <c r="O7" s="11">
+      <c r="O7" s="5">
         <f t="shared" si="7"/>
         <v>-0.11920361114432618</v>
       </c>
       <c r="P7">
         <f t="shared" si="8"/>
-        <v>48</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -2616,13 +2577,13 @@
         <f t="shared" si="0"/>
         <v>-236476.69000000996</v>
       </c>
-      <c r="E8" s="10">
-        <f t="shared" si="1"/>
+      <c r="E8" s="5">
+        <f t="shared" si="2"/>
         <v>-0.15235918433091292</v>
       </c>
       <c r="F8">
-        <f t="shared" si="2"/>
-        <v>51</v>
+        <f t="shared" si="3"/>
+        <v>28</v>
       </c>
       <c r="G8">
         <v>1590700</v>
@@ -2631,7 +2592,7 @@
         <v>1383905.98999999</v>
       </c>
       <c r="I8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-206794.01000001002</v>
       </c>
       <c r="J8" s="5">
@@ -2640,7 +2601,7 @@
       </c>
       <c r="K8">
         <f t="shared" si="5"/>
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="L8">
         <v>1579300</v>
@@ -2652,13 +2613,13 @@
         <f t="shared" si="6"/>
         <v>-241564.68000000995</v>
       </c>
-      <c r="O8" s="11">
+      <c r="O8" s="5">
         <f t="shared" si="7"/>
         <v>-0.15295680364719175</v>
       </c>
       <c r="P8">
         <f t="shared" si="8"/>
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -2675,13 +2636,13 @@
         <f t="shared" si="0"/>
         <v>-396574.72000000067</v>
       </c>
-      <c r="E9" s="10">
-        <f t="shared" si="1"/>
+      <c r="E9" s="5">
+        <f t="shared" si="2"/>
         <v>-4.2417130511048909E-2</v>
       </c>
       <c r="F9">
-        <f t="shared" si="2"/>
-        <v>36</v>
+        <f t="shared" si="3"/>
+        <v>37</v>
       </c>
       <c r="G9">
         <v>11073700</v>
@@ -2690,7 +2651,7 @@
         <v>9929059.5199999996</v>
       </c>
       <c r="I9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-1144640.4800000004</v>
       </c>
       <c r="J9" s="5">
@@ -2699,7 +2660,7 @@
       </c>
       <c r="K9">
         <f t="shared" si="5"/>
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="L9">
         <v>10790500</v>
@@ -2711,13 +2672,13 @@
         <f t="shared" si="6"/>
         <v>-796900.47000000998</v>
       </c>
-      <c r="O9" s="11">
+      <c r="O9" s="5">
         <f t="shared" si="7"/>
         <v>-7.3852043000788653E-2</v>
       </c>
       <c r="P9">
         <f t="shared" si="8"/>
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -2734,13 +2695,13 @@
         <f t="shared" si="0"/>
         <v>-36209.630000000005</v>
       </c>
-      <c r="E10" s="10">
-        <f t="shared" si="1"/>
+      <c r="E10" s="5">
+        <f t="shared" si="2"/>
         <v>-8.1681998646514792E-2</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
-        <v>46</v>
+        <f t="shared" si="3"/>
+        <v>34</v>
       </c>
       <c r="G10">
         <v>495200</v>
@@ -2749,7 +2710,7 @@
         <v>467907.84000000003</v>
       </c>
       <c r="I10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-27292.159999999974</v>
       </c>
       <c r="J10" s="5">
@@ -2758,7 +2719,7 @@
       </c>
       <c r="K10">
         <f t="shared" si="5"/>
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="L10">
         <v>487500</v>
@@ -2770,13 +2731,13 @@
         <f t="shared" si="6"/>
         <v>-9181.0800000000163</v>
       </c>
-      <c r="O10" s="11">
+      <c r="O10" s="5">
         <f t="shared" si="7"/>
         <v>-1.883298461538465E-2</v>
       </c>
       <c r="P10">
         <f t="shared" si="8"/>
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -2793,31 +2754,31 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="5" t="str">
+        <f>IF(B11&lt;&gt;0, (C11-B11)/B11, IF(C11=0, "",))</f>
+        <v/>
+      </c>
+      <c r="F11" t="e">
+        <f>IF(E11&lt;&gt;0, RANK(E11, $E$2:$E$52))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J11" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K11">
+      <c r="K11" t="b">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11">
         <v>375000</v>
@@ -2829,13 +2790,13 @@
         <f t="shared" si="6"/>
         <v>-311228.08999999997</v>
       </c>
-      <c r="O11" s="11">
+      <c r="O11" s="5">
         <f t="shared" si="7"/>
         <v>-0.82994157333333329</v>
       </c>
       <c r="P11">
         <f t="shared" si="8"/>
-        <v>51</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -2852,13 +2813,13 @@
         <f t="shared" si="0"/>
         <v>-214304.66999999993</v>
       </c>
-      <c r="E12" s="10">
-        <f t="shared" si="1"/>
+      <c r="E12" s="5">
+        <f t="shared" si="2"/>
         <v>-5.0060657805601608E-2</v>
       </c>
       <c r="F12">
-        <f t="shared" si="2"/>
-        <v>39</v>
+        <f t="shared" ref="F12:F52" si="9">IF(E12&lt;&gt;0, RANK(E12, $E$2:$E$52))</f>
+        <v>36</v>
       </c>
       <c r="G12">
         <v>4700400</v>
@@ -2867,7 +2828,7 @@
         <v>4205555.5999999996</v>
       </c>
       <c r="I12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-494844.40000000037</v>
       </c>
       <c r="J12" s="5">
@@ -2876,7 +2837,7 @@
       </c>
       <c r="K12">
         <f t="shared" si="5"/>
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="L12">
         <v>4677800</v>
@@ -2888,13 +2849,13 @@
         <f t="shared" si="6"/>
         <v>-306086.86000000034</v>
       </c>
-      <c r="O12" s="11">
+      <c r="O12" s="5">
         <f t="shared" si="7"/>
         <v>-6.5433934755654441E-2</v>
       </c>
       <c r="P12">
         <f t="shared" si="8"/>
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -2911,13 +2872,13 @@
         <f t="shared" si="0"/>
         <v>-75511.669999999925</v>
       </c>
-      <c r="E13" s="10">
-        <f t="shared" si="1"/>
+      <c r="E13" s="5">
+        <f t="shared" si="2"/>
         <v>-1.2912833886247806E-2</v>
       </c>
       <c r="F13">
-        <f t="shared" si="2"/>
-        <v>19</v>
+        <f t="shared" si="9"/>
+        <v>16</v>
       </c>
       <c r="G13">
         <v>6223700</v>
@@ -2926,7 +2887,7 @@
         <v>5909077.9399999902</v>
       </c>
       <c r="I13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-314622.06000000983</v>
       </c>
       <c r="J13" s="5">
@@ -2935,7 +2896,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="5"/>
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="L13">
         <v>6207300</v>
@@ -2947,13 +2908,13 @@
         <f t="shared" si="6"/>
         <v>-150323.33000000007</v>
       </c>
-      <c r="O13" s="11">
+      <c r="O13" s="5">
         <f t="shared" si="7"/>
         <v>-2.4217184605222895E-2</v>
       </c>
       <c r="P13">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -2970,13 +2931,13 @@
         <f t="shared" si="0"/>
         <v>-6982.6300000000047</v>
       </c>
-      <c r="E14" s="10">
-        <f t="shared" si="1"/>
+      <c r="E14" s="5">
+        <f t="shared" si="2"/>
         <v>-1.3637949218750009E-2</v>
       </c>
       <c r="F14">
-        <f t="shared" si="2"/>
-        <v>22</v>
+        <f t="shared" si="9"/>
+        <v>19</v>
       </c>
       <c r="G14">
         <v>530500</v>
@@ -2985,7 +2946,7 @@
         <v>524402.98</v>
       </c>
       <c r="I14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-6097.0200000000186</v>
       </c>
       <c r="J14" s="5">
@@ -2994,7 +2955,7 @@
       </c>
       <c r="K14">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="L14">
         <v>526200</v>
@@ -3006,13 +2967,13 @@
         <f t="shared" si="6"/>
         <v>-21210.119999999995</v>
       </c>
-      <c r="O14" s="11">
+      <c r="O14" s="5">
         <f t="shared" si="7"/>
         <v>-4.0308095781071827E-2</v>
       </c>
       <c r="P14">
         <f t="shared" si="8"/>
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -3029,12 +2990,12 @@
         <f t="shared" si="0"/>
         <v>496819.90000000596</v>
       </c>
-      <c r="E15" s="10">
-        <f t="shared" si="1"/>
+      <c r="E15" s="5">
+        <f t="shared" si="2"/>
         <v>3.1837408866824991E-3</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="G15">
@@ -3044,7 +3005,7 @@
         <v>175966389.24999899</v>
       </c>
       <c r="I15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-8201410.7500010133</v>
       </c>
       <c r="J15" s="5">
@@ -3053,7 +3014,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="5"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L15">
         <v>188953500</v>
@@ -3065,13 +3026,13 @@
         <f t="shared" si="6"/>
         <v>-4502589.1500009894</v>
       </c>
-      <c r="O15" s="11">
+      <c r="O15" s="5">
         <f t="shared" si="7"/>
         <v>-2.3829085727446114E-2</v>
       </c>
       <c r="P15">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -3088,13 +3049,13 @@
         <f t="shared" si="0"/>
         <v>-78219.540000010282</v>
       </c>
-      <c r="E16" s="10">
-        <f t="shared" si="1"/>
+      <c r="E16" s="5">
+        <f t="shared" si="2"/>
         <v>-1.1850188616360429E-2</v>
       </c>
       <c r="F16">
-        <f t="shared" si="2"/>
-        <v>15</v>
+        <f t="shared" si="9"/>
+        <v>12</v>
       </c>
       <c r="G16">
         <v>7352500</v>
@@ -3103,7 +3064,7 @@
         <v>7350464.0800000001</v>
       </c>
       <c r="I16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-2035.9199999999255</v>
       </c>
       <c r="J16" s="5">
@@ -3112,7 +3073,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="L16">
         <v>7397200</v>
@@ -3124,13 +3085,13 @@
         <f t="shared" si="6"/>
         <v>-107</v>
       </c>
-      <c r="O16" s="11">
+      <c r="O16" s="5">
         <f t="shared" si="7"/>
         <v>-1.4464932677229222E-5</v>
       </c>
       <c r="P16">
         <f t="shared" si="8"/>
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -3147,13 +3108,13 @@
         <f t="shared" si="0"/>
         <v>-421319.94999999925</v>
       </c>
-      <c r="E17" s="10">
-        <f t="shared" si="1"/>
+      <c r="E17" s="5">
+        <f t="shared" si="2"/>
         <v>-2.8351094826658003E-2</v>
       </c>
       <c r="F17">
-        <f t="shared" si="2"/>
-        <v>31</v>
+        <f t="shared" si="9"/>
+        <v>28</v>
       </c>
       <c r="G17">
         <v>15309700</v>
@@ -3162,7 +3123,7 @@
         <v>14645233.51</v>
       </c>
       <c r="I17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-664466.49000000022</v>
       </c>
       <c r="J17" s="5">
@@ -3171,7 +3132,7 @@
       </c>
       <c r="K17">
         <f t="shared" si="5"/>
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="L17">
         <v>15311800</v>
@@ -3183,13 +3144,13 @@
         <f t="shared" si="6"/>
         <v>-965742.96000000089</v>
       </c>
-      <c r="O17" s="11">
+      <c r="O17" s="5">
         <f t="shared" si="7"/>
         <v>-6.3071811282801551E-2</v>
       </c>
       <c r="P17">
         <f t="shared" si="8"/>
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -3206,13 +3167,13 @@
         <f t="shared" si="0"/>
         <v>-149396.10000000987</v>
       </c>
-      <c r="E18" s="10">
-        <f t="shared" si="1"/>
+      <c r="E18" s="5">
+        <f t="shared" si="2"/>
         <v>-5.4037002206391245E-2</v>
       </c>
       <c r="F18">
-        <f t="shared" si="2"/>
-        <v>40</v>
+        <f t="shared" si="9"/>
+        <v>37</v>
       </c>
       <c r="G18">
         <v>2861000</v>
@@ -3221,7 +3182,7 @@
         <v>2671745.94</v>
       </c>
       <c r="I18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="J18" s="5">
@@ -3230,7 +3191,7 @@
       </c>
       <c r="K18">
         <f t="shared" si="5"/>
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="L18">
         <v>2910600</v>
@@ -3242,13 +3203,13 @@
         <f t="shared" si="6"/>
         <v>-374962.91000000015</v>
       </c>
-      <c r="O18" s="11">
+      <c r="O18" s="5">
         <f t="shared" si="7"/>
         <v>-0.12882667147667154</v>
       </c>
       <c r="P18">
         <f t="shared" si="8"/>
-        <v>49</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -3265,13 +3226,13 @@
         <f t="shared" si="0"/>
         <v>-376336.80000001006</v>
       </c>
-      <c r="E19" s="10">
-        <f t="shared" si="1"/>
+      <c r="E19" s="5">
+        <f t="shared" si="2"/>
         <v>-4.258504294298146E-2</v>
       </c>
       <c r="F19">
-        <f t="shared" si="2"/>
-        <v>37</v>
+        <f t="shared" si="9"/>
+        <v>34</v>
       </c>
       <c r="G19">
         <v>9713300</v>
@@ -3280,7 +3241,7 @@
         <v>8991707.2399999909</v>
       </c>
       <c r="I19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-721592.76000000909</v>
       </c>
       <c r="J19" s="5">
@@ -3289,7 +3250,7 @@
       </c>
       <c r="K19">
         <f t="shared" si="5"/>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="L19">
         <v>9343000</v>
@@ -3301,13 +3262,13 @@
         <f t="shared" si="6"/>
         <v>-576344.08999999985</v>
       </c>
-      <c r="O19" s="11">
+      <c r="O19" s="5">
         <f t="shared" si="7"/>
         <v>-6.1687262121374278E-2</v>
       </c>
       <c r="P19">
         <f t="shared" si="8"/>
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -3324,13 +3285,13 @@
         <f t="shared" si="0"/>
         <v>-1539.8400010019541</v>
       </c>
-      <c r="E20" s="9">
-        <f>D20/B20</f>
+      <c r="E20" s="5">
+        <f t="shared" si="2"/>
         <v>-1.2379538203300809E-5</v>
       </c>
       <c r="F20">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f t="shared" si="9"/>
+        <v>3</v>
       </c>
       <c r="G20">
         <v>131849400</v>
@@ -3339,7 +3300,7 @@
         <v>131839624.37</v>
       </c>
       <c r="I20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-9775.6299999952316</v>
       </c>
       <c r="J20" s="5">
@@ -3348,7 +3309,7 @@
       </c>
       <c r="K20">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="L20">
         <v>130621400</v>
@@ -3360,13 +3321,13 @@
         <f t="shared" si="6"/>
         <v>-116.46000100672245</v>
       </c>
-      <c r="O20" s="11">
+      <c r="O20" s="5">
         <f t="shared" si="7"/>
         <v>-8.9158438821450736E-7</v>
       </c>
       <c r="P20">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -3383,13 +3344,13 @@
         <f t="shared" si="0"/>
         <v>-1923512.4500000998</v>
       </c>
-      <c r="E21" s="10">
-        <f t="shared" si="1"/>
+      <c r="E21" s="5">
+        <f t="shared" si="2"/>
         <v>-7.9052463618023094E-2</v>
       </c>
       <c r="F21">
-        <f t="shared" si="2"/>
-        <v>43</v>
+        <f t="shared" si="9"/>
+        <v>40</v>
       </c>
       <c r="G21">
         <v>24497400</v>
@@ -3398,7 +3359,7 @@
         <v>22655993.629999999</v>
       </c>
       <c r="I21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-1841406.370000001</v>
       </c>
       <c r="J21" s="5">
@@ -3407,7 +3368,7 @@
       </c>
       <c r="K21">
         <f t="shared" si="5"/>
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="L21">
         <v>24323000</v>
@@ -3419,13 +3380,13 @@
         <f t="shared" si="6"/>
         <v>-888926.91000010073</v>
       </c>
-      <c r="O21" s="11">
+      <c r="O21" s="5">
         <f t="shared" si="7"/>
         <v>-3.6546762734864152E-2</v>
       </c>
       <c r="P21">
         <f t="shared" si="8"/>
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -3442,13 +3403,13 @@
         <f t="shared" si="0"/>
         <v>-153660.12000009976</v>
       </c>
-      <c r="E22" s="10">
-        <f t="shared" si="1"/>
+      <c r="E22" s="5">
+        <f t="shared" si="2"/>
         <v>-1.3285502334437123E-2</v>
       </c>
       <c r="F22">
-        <f t="shared" si="2"/>
-        <v>20</v>
+        <f t="shared" si="9"/>
+        <v>17</v>
       </c>
       <c r="G22">
         <v>11980700</v>
@@ -3457,7 +3418,7 @@
         <v>11791977.9699999</v>
       </c>
       <c r="I22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-188722.03000009991</v>
       </c>
       <c r="J22" s="5">
@@ -3466,7 +3427,7 @@
       </c>
       <c r="K22">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="L22">
         <v>11935200</v>
@@ -3478,13 +3439,13 @@
         <f t="shared" si="6"/>
         <v>-745.23000000044703</v>
       </c>
-      <c r="O22" s="11">
+      <c r="O22" s="5">
         <f t="shared" si="7"/>
         <v>-6.2439674240938325E-5</v>
       </c>
       <c r="P22">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -3501,13 +3462,13 @@
         <f t="shared" si="0"/>
         <v>-825956.59000010043</v>
       </c>
-      <c r="E23" s="10">
-        <f t="shared" si="1"/>
+      <c r="E23" s="5">
+        <f t="shared" si="2"/>
         <v>-3.9590110100806722E-2</v>
       </c>
       <c r="F23">
-        <f t="shared" si="2"/>
-        <v>34</v>
+        <f t="shared" si="9"/>
+        <v>31</v>
       </c>
       <c r="G23">
         <v>22683800</v>
@@ -3516,7 +3477,7 @@
         <v>21722126.219999898</v>
       </c>
       <c r="I23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-961673.78000010177</v>
       </c>
       <c r="J23" s="5">
@@ -3525,7 +3486,7 @@
       </c>
       <c r="K23">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="L23">
         <v>23220300</v>
@@ -3537,13 +3498,13 @@
         <f t="shared" si="6"/>
         <v>-601242.55999999866</v>
       </c>
-      <c r="O23" s="11">
+      <c r="O23" s="5">
         <f t="shared" si="7"/>
         <v>-2.5892971236375011E-2</v>
       </c>
       <c r="P23">
         <f t="shared" si="8"/>
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -3560,13 +3521,13 @@
         <f t="shared" si="0"/>
         <v>-12230.810000000056</v>
       </c>
-      <c r="E24" s="10">
-        <f t="shared" si="1"/>
+      <c r="E24" s="5">
+        <f t="shared" si="2"/>
         <v>-1.3334943305713101E-2</v>
       </c>
       <c r="F24">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f t="shared" si="9"/>
+        <v>18</v>
       </c>
       <c r="G24">
         <v>1112700</v>
@@ -3575,7 +3536,7 @@
         <v>1067214.42</v>
       </c>
       <c r="I24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="J24" s="5">
@@ -3584,7 +3545,7 @@
       </c>
       <c r="K24">
         <f t="shared" si="5"/>
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="L24">
         <v>1112600</v>
@@ -3596,13 +3557,13 @@
         <f t="shared" si="6"/>
         <v>-72.879999999888241</v>
       </c>
-      <c r="O24" s="11">
+      <c r="O24" s="5">
         <f t="shared" si="7"/>
         <v>-6.5504224339284781E-5</v>
       </c>
       <c r="P24">
         <f t="shared" si="8"/>
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -3619,13 +3580,13 @@
         <f t="shared" si="0"/>
         <v>-4950.4699999999721</v>
       </c>
-      <c r="E25" s="10">
-        <f t="shared" si="1"/>
+      <c r="E25" s="5">
+        <f t="shared" si="2"/>
         <v>-1.0226130964676661E-2</v>
       </c>
       <c r="F25">
-        <f t="shared" si="2"/>
-        <v>14</v>
+        <f t="shared" si="9"/>
+        <v>11</v>
       </c>
       <c r="G25">
         <v>505200</v>
@@ -3634,7 +3595,7 @@
         <v>497194.20999999897</v>
       </c>
       <c r="I25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="J25" s="5">
@@ -3643,7 +3604,7 @@
       </c>
       <c r="K25">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="L25">
         <v>496500</v>
@@ -3655,13 +3616,13 @@
         <f t="shared" si="6"/>
         <v>-1724.9000000000233</v>
       </c>
-      <c r="O25" s="11">
+      <c r="O25" s="5">
         <f t="shared" si="7"/>
         <v>-3.4741188318228064E-3</v>
       </c>
       <c r="P25">
         <f t="shared" si="8"/>
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -3678,13 +3639,13 @@
         <f t="shared" si="0"/>
         <v>-447839.91999999993</v>
       </c>
-      <c r="E26" s="10">
-        <f t="shared" si="1"/>
+      <c r="E26" s="5">
+        <f t="shared" si="2"/>
         <v>-8.5306091660634673E-2</v>
       </c>
       <c r="F26">
-        <f t="shared" si="2"/>
-        <v>47</v>
+        <f t="shared" si="9"/>
+        <v>44</v>
       </c>
       <c r="G26">
         <v>5442200</v>
@@ -3693,7 +3654,7 @@
         <v>5122329.02999999</v>
       </c>
       <c r="I26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-319870.97000000998</v>
       </c>
       <c r="J26" s="5">
@@ -3702,7 +3663,7 @@
       </c>
       <c r="K26">
         <f t="shared" si="5"/>
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="L26">
         <v>5430700</v>
@@ -3714,13 +3675,13 @@
         <f t="shared" si="6"/>
         <v>-313464.79000000004</v>
       </c>
-      <c r="O26" s="11">
+      <c r="O26" s="5">
         <f t="shared" si="7"/>
         <v>-5.7720881286022069E-2</v>
       </c>
       <c r="P26">
         <f t="shared" si="8"/>
-        <v>39</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -3737,31 +3698,31 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="5" t="str">
+        <f>IF(B27&lt;&gt;0, (C27-B27)/B27, IF(C27=0, "",))</f>
+        <v/>
+      </c>
+      <c r="F27" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J27" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K27">
+      <c r="K27" t="b">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L27">
         <v>0</v>
@@ -3773,13 +3734,13 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O27" s="11">
+      <c r="O27" s="5">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P27">
+      <c r="P27" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -3796,13 +3757,13 @@
         <f t="shared" si="0"/>
         <v>-132457.97999999998</v>
       </c>
-      <c r="E28" s="10">
-        <f t="shared" si="1"/>
+      <c r="E28" s="5">
+        <f t="shared" si="2"/>
         <v>-9.5782760864849215E-2</v>
       </c>
       <c r="F28">
-        <f t="shared" si="2"/>
-        <v>49</v>
+        <f t="shared" si="9"/>
+        <v>46</v>
       </c>
       <c r="G28">
         <v>1545700</v>
@@ -3811,7 +3772,7 @@
         <v>1281335.23</v>
       </c>
       <c r="I28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-264364.77</v>
       </c>
       <c r="J28" s="5">
@@ -3820,7 +3781,7 @@
       </c>
       <c r="K28">
         <f t="shared" si="5"/>
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="L28">
         <v>1525900</v>
@@ -3832,13 +3793,13 @@
         <f t="shared" si="6"/>
         <v>-132614.93999999994</v>
       </c>
-      <c r="O28" s="11">
+      <c r="O28" s="5">
         <f t="shared" si="7"/>
         <v>-8.6909325643882263E-2</v>
       </c>
       <c r="P28">
         <f t="shared" si="8"/>
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -3855,13 +3816,13 @@
         <f t="shared" si="0"/>
         <v>-37915.290000000037</v>
       </c>
-      <c r="E29" s="10">
-        <f t="shared" si="1"/>
+      <c r="E29" s="5">
+        <f t="shared" si="2"/>
         <v>-1.4800253727847622E-2</v>
       </c>
       <c r="F29">
-        <f t="shared" si="2"/>
-        <v>24</v>
+        <f t="shared" si="9"/>
+        <v>21</v>
       </c>
       <c r="G29">
         <v>2779500</v>
@@ -3870,7 +3831,7 @@
         <v>2665264.4399999902</v>
       </c>
       <c r="I29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-114235.56000000983</v>
       </c>
       <c r="J29" s="5">
@@ -3879,7 +3840,7 @@
       </c>
       <c r="K29">
         <f t="shared" si="5"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="L29">
         <v>2889900</v>
@@ -3891,13 +3852,13 @@
         <f t="shared" si="6"/>
         <v>-35.330000000074506</v>
       </c>
-      <c r="O29" s="11">
+      <c r="O29" s="5">
         <f t="shared" si="7"/>
         <v>-1.2225336516860273E-5</v>
       </c>
       <c r="P29">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -3914,13 +3875,13 @@
         <f t="shared" si="0"/>
         <v>-101705.90000000037</v>
       </c>
-      <c r="E30" s="10">
-        <f t="shared" si="1"/>
+      <c r="E30" s="5">
+        <f t="shared" si="2"/>
         <v>-8.3831374359143746E-3</v>
       </c>
       <c r="F30">
-        <f t="shared" si="2"/>
-        <v>12</v>
+        <f t="shared" si="9"/>
+        <v>9</v>
       </c>
       <c r="G30">
         <v>12735900</v>
@@ -3929,7 +3890,7 @@
         <v>12685514.279999901</v>
       </c>
       <c r="I30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-50385.720000099391</v>
       </c>
       <c r="J30" s="5">
@@ -3938,7 +3899,7 @@
       </c>
       <c r="K30">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="L30">
         <v>12861300</v>
@@ -3950,13 +3911,13 @@
         <f t="shared" si="6"/>
         <v>-35290.390000000596</v>
       </c>
-      <c r="O30" s="11">
+      <c r="O30" s="5">
         <f t="shared" si="7"/>
         <v>-2.7439209100169185E-3</v>
       </c>
       <c r="P30">
         <f t="shared" si="8"/>
-        <v>16</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -3973,13 +3934,13 @@
         <f t="shared" si="0"/>
         <v>-24772.310000000056</v>
       </c>
-      <c r="E31" s="10">
-        <f t="shared" si="1"/>
+      <c r="E31" s="5">
+        <f t="shared" si="2"/>
         <v>-1.4030533529678329E-2</v>
       </c>
       <c r="F31">
-        <f t="shared" si="2"/>
-        <v>23</v>
+        <f t="shared" si="9"/>
+        <v>20</v>
       </c>
       <c r="G31">
         <v>1823300</v>
@@ -3988,7 +3949,7 @@
         <v>1762676.85</v>
       </c>
       <c r="I31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-60623.149999999907</v>
       </c>
       <c r="J31" s="5">
@@ -3997,7 +3958,7 @@
       </c>
       <c r="K31">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="L31">
         <v>1870700</v>
@@ -4009,13 +3970,13 @@
         <f t="shared" si="6"/>
         <v>-69308.659999999916</v>
       </c>
-      <c r="O31" s="11">
+      <c r="O31" s="5">
         <f t="shared" si="7"/>
         <v>-3.7049585716576634E-2</v>
       </c>
       <c r="P31">
         <f t="shared" si="8"/>
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -4032,13 +3993,13 @@
         <f t="shared" si="0"/>
         <v>-73762.280000009574</v>
       </c>
-      <c r="E32" s="10">
-        <f t="shared" si="1"/>
+      <c r="E32" s="5">
+        <f t="shared" si="2"/>
         <v>-1.2294942827617691E-2</v>
       </c>
       <c r="F32">
-        <f t="shared" si="2"/>
-        <v>16</v>
+        <f t="shared" si="9"/>
+        <v>13</v>
       </c>
       <c r="G32">
         <v>6195500</v>
@@ -4047,7 +4008,7 @@
         <v>6084985.4699999997</v>
       </c>
       <c r="I32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-110514.53000000026</v>
       </c>
       <c r="J32" s="5">
@@ -4056,7 +4017,7 @@
       </c>
       <c r="K32">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L32">
         <v>6157400</v>
@@ -4068,13 +4029,13 @@
         <f t="shared" si="6"/>
         <v>-169827.98000000045</v>
       </c>
-      <c r="O32" s="11">
+      <c r="O32" s="5">
         <f t="shared" si="7"/>
         <v>-2.7581118653977402E-2</v>
       </c>
       <c r="P32">
         <f t="shared" si="8"/>
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -4091,13 +4052,13 @@
         <f t="shared" si="0"/>
         <v>-7418835.2699990273</v>
       </c>
-      <c r="E33" s="10">
-        <f t="shared" si="1"/>
+      <c r="E33" s="5">
+        <f t="shared" si="2"/>
         <v>-7.9969930789269058E-3</v>
       </c>
       <c r="F33">
-        <f t="shared" si="2"/>
-        <v>11</v>
+        <f t="shared" si="9"/>
+        <v>8</v>
       </c>
       <c r="G33">
         <v>979671000</v>
@@ -4106,7 +4067,7 @@
         <v>977068513.48000002</v>
       </c>
       <c r="I33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-2602486.5199999809</v>
       </c>
       <c r="J33" s="5">
@@ -4115,7 +4076,7 @@
       </c>
       <c r="K33">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="L33">
         <v>989572899.99999905</v>
@@ -4127,13 +4088,13 @@
         <f t="shared" si="6"/>
         <v>-5456610.5900000334</v>
       </c>
-      <c r="O33" s="11">
+      <c r="O33" s="5">
         <f t="shared" si="7"/>
         <v>-5.5141067323084929E-3</v>
       </c>
       <c r="P33">
         <f t="shared" si="8"/>
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -4147,16 +4108,16 @@
         <v>4109958.22</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34:D65" si="9">C34-B34</f>
+        <f t="shared" ref="D34:D52" si="10">C34-B34</f>
         <v>-79341.779999999795</v>
       </c>
-      <c r="E34" s="10">
-        <f t="shared" ref="E34:E52" si="10">IF(B34&lt;&gt;0, (C34-B34)/B34, IF(C34=0, 0, ""))</f>
+      <c r="E34" s="5">
+        <f t="shared" si="2"/>
         <v>-1.8939149738619768E-2</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34:F65" si="11">IF(E34&lt;&gt;"", RANK(E34, $E$2:$E$52), "")</f>
-        <v>26</v>
+        <f t="shared" si="9"/>
+        <v>23</v>
       </c>
       <c r="G34">
         <v>4350600</v>
@@ -4165,16 +4126,16 @@
         <v>4137588.7699999898</v>
       </c>
       <c r="I34">
-        <f t="shared" ref="I34:I65" si="12">H34-G34</f>
+        <f t="shared" ref="I34:I52" si="11">H34-G34</f>
         <v>-213011.23000001023</v>
       </c>
       <c r="J34" s="5">
-        <f t="shared" ref="J34:J52" si="13">IF(G34&lt;&gt;0, (H34-G34)/G34, IF(H34=0, 0, ""))</f>
+        <f t="shared" si="4"/>
         <v>-4.8961345561534093E-2</v>
       </c>
       <c r="K34">
         <f t="shared" si="5"/>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L34">
         <v>4345600</v>
@@ -4186,13 +4147,13 @@
         <f t="shared" si="6"/>
         <v>-115798.49000000022</v>
       </c>
-      <c r="O34" s="11">
+      <c r="O34" s="5">
         <f t="shared" si="7"/>
         <v>-2.6647296115611244E-2</v>
       </c>
       <c r="P34">
         <f t="shared" si="8"/>
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -4206,34 +4167,34 @@
         <v>0</v>
       </c>
       <c r="D35">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="5" t="str">
+        <f>IF(B35&lt;&gt;0, (C35-B35)/B35, IF(C35=0, "",))</f>
+        <v/>
+      </c>
+      <c r="F35" t="e">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="E35" s="10">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F35">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
         <f t="shared" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J35" s="5">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="K35">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K35" t="b">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L35">
         <v>0</v>
@@ -4245,13 +4206,13 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O35" s="11">
+      <c r="O35" s="5">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P35">
+      <c r="P35" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -4265,16 +4226,16 @@
         <v>735423.27999999898</v>
       </c>
       <c r="D36">
+        <f t="shared" si="10"/>
+        <v>-62776.72000000102</v>
+      </c>
+      <c r="E36" s="5">
+        <f t="shared" si="2"/>
+        <v>-7.8647857679780775E-2</v>
+      </c>
+      <c r="F36">
         <f t="shared" si="9"/>
-        <v>-62776.72000000102</v>
-      </c>
-      <c r="E36" s="10">
-        <f t="shared" si="10"/>
-        <v>-7.8647857679780775E-2</v>
-      </c>
-      <c r="F36">
-        <f t="shared" si="11"/>
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G36">
         <v>898700</v>
@@ -4283,16 +4244,16 @@
         <v>740966.94999999902</v>
       </c>
       <c r="I36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-157733.05000000098</v>
       </c>
       <c r="J36" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>-0.17551246244575608</v>
       </c>
       <c r="K36">
         <f t="shared" si="5"/>
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="L36">
         <v>878300</v>
@@ -4304,13 +4265,13 @@
         <f t="shared" si="6"/>
         <v>-101084.71000000101</v>
       </c>
-      <c r="O36" s="11">
+      <c r="O36" s="5">
         <f t="shared" si="7"/>
         <v>-0.11509132414892521</v>
       </c>
       <c r="P36">
         <f t="shared" si="8"/>
-        <v>47</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -4324,16 +4285,16 @@
         <v>2005447.73999999</v>
       </c>
       <c r="D37">
+        <f t="shared" si="10"/>
+        <v>-82352.260000010021</v>
+      </c>
+      <c r="E37" s="5">
+        <f t="shared" si="2"/>
+        <v>-3.9444515758219188E-2</v>
+      </c>
+      <c r="F37">
         <f t="shared" si="9"/>
-        <v>-82352.260000010021</v>
-      </c>
-      <c r="E37" s="10">
-        <f t="shared" si="10"/>
-        <v>-3.9444515758219188E-2</v>
-      </c>
-      <c r="F37">
-        <f t="shared" si="11"/>
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G37">
         <v>2229200</v>
@@ -4342,16 +4303,16 @@
         <v>2118943.21</v>
       </c>
       <c r="I37">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-110256.79000000004</v>
       </c>
       <c r="J37" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>-4.9460250314014013E-2</v>
       </c>
       <c r="K37">
         <f t="shared" si="5"/>
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="L37">
         <v>2296900</v>
@@ -4363,13 +4324,13 @@
         <f t="shared" si="6"/>
         <v>-188181.66000000015</v>
       </c>
-      <c r="O37" s="11">
+      <c r="O37" s="5">
         <f t="shared" si="7"/>
         <v>-8.1928538464887526E-2</v>
       </c>
       <c r="P37">
         <f t="shared" si="8"/>
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -4383,16 +4344,16 @@
         <v>838669.82</v>
       </c>
       <c r="D38">
+        <f t="shared" si="10"/>
+        <v>-16630.180000000051</v>
+      </c>
+      <c r="E38" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.9443680579913542E-2</v>
+      </c>
+      <c r="F38">
         <f t="shared" si="9"/>
-        <v>-16630.180000000051</v>
-      </c>
-      <c r="E38" s="10">
-        <f t="shared" si="10"/>
-        <v>-1.9443680579913542E-2</v>
-      </c>
-      <c r="F38">
-        <f t="shared" si="11"/>
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G38">
         <v>792800</v>
@@ -4401,16 +4362,16 @@
         <v>753451.96</v>
       </c>
       <c r="I38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-39348.040000000037</v>
       </c>
       <c r="J38" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>-4.9631735620585316E-2</v>
       </c>
       <c r="K38">
         <f t="shared" si="5"/>
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="L38">
         <v>777800</v>
@@ -4422,13 +4383,13 @@
         <f t="shared" si="6"/>
         <v>-136.73999999999069</v>
       </c>
-      <c r="O38" s="11">
+      <c r="O38" s="5">
         <f t="shared" si="7"/>
         <v>-1.7580354847003174E-4</v>
       </c>
       <c r="P38">
         <f t="shared" si="8"/>
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -4442,16 +4403,16 @@
         <v>813108.87</v>
       </c>
       <c r="D39">
+        <f t="shared" si="10"/>
+        <v>-70791.13</v>
+      </c>
+      <c r="E39" s="5">
+        <f t="shared" si="2"/>
+        <v>-8.008952370177623E-2</v>
+      </c>
+      <c r="F39">
         <f t="shared" si="9"/>
-        <v>-70791.13</v>
-      </c>
-      <c r="E39" s="10">
-        <f t="shared" si="10"/>
-        <v>-8.008952370177623E-2</v>
-      </c>
-      <c r="F39">
-        <f t="shared" si="11"/>
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G39">
         <v>1294400</v>
@@ -4460,16 +4421,16 @@
         <v>1114242.27999999</v>
       </c>
       <c r="I39">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-180157.72000000998</v>
       </c>
       <c r="J39" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>-0.13918241656366656</v>
       </c>
       <c r="K39">
         <f t="shared" si="5"/>
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="L39">
         <v>1759500</v>
@@ -4481,13 +4442,13 @@
         <f t="shared" si="6"/>
         <v>-79036.1300000099</v>
       </c>
-      <c r="O39" s="11">
+      <c r="O39" s="5">
         <f t="shared" si="7"/>
         <v>-4.4919653310605226E-2</v>
       </c>
       <c r="P39">
         <f t="shared" si="8"/>
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -4501,16 +4462,16 @@
         <v>37565141.859999903</v>
       </c>
       <c r="D40">
+        <f t="shared" si="10"/>
+        <v>-816758.14000009745</v>
+      </c>
+      <c r="E40" s="5">
+        <f t="shared" si="2"/>
+        <v>-2.1279773539092578E-2</v>
+      </c>
+      <c r="F40">
         <f t="shared" si="9"/>
-        <v>-816758.14000009745</v>
-      </c>
-      <c r="E40" s="10">
-        <f t="shared" si="10"/>
-        <v>-2.1279773539092578E-2</v>
-      </c>
-      <c r="F40">
-        <f t="shared" si="11"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G40">
         <v>39964900</v>
@@ -4519,16 +4480,16 @@
         <v>38095240.189999901</v>
       </c>
       <c r="I40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-1869659.8100000992</v>
       </c>
       <c r="J40" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>-4.6782546934937892E-2</v>
       </c>
       <c r="K40">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="L40">
         <v>40216700</v>
@@ -4540,13 +4501,13 @@
         <f t="shared" si="6"/>
         <v>-610436.29000010341</v>
       </c>
-      <c r="O40" s="11">
+      <c r="O40" s="5">
         <f t="shared" si="7"/>
         <v>-1.5178676768608648E-2</v>
       </c>
       <c r="P40">
         <f t="shared" si="8"/>
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -4560,16 +4521,16 @@
         <v>4409060.2099999897</v>
       </c>
       <c r="D41">
+        <f t="shared" si="10"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="E41" s="5">
+        <f t="shared" si="2"/>
+        <v>-4.0110550149132493E-2</v>
+      </c>
+      <c r="F41">
         <f t="shared" si="9"/>
-        <v>-184239.79000001028</v>
-      </c>
-      <c r="E41" s="10">
-        <f t="shared" si="10"/>
-        <v>-4.0110550149132493E-2</v>
-      </c>
-      <c r="F41">
-        <f t="shared" si="11"/>
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G41">
         <v>5089500</v>
@@ -4578,16 +4539,16 @@
         <v>4956043.6699999897</v>
       </c>
       <c r="I41">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="J41" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>-2.6221894095689226E-2</v>
       </c>
       <c r="K41">
         <f t="shared" si="5"/>
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="L41">
         <v>4799900</v>
@@ -4599,13 +4560,13 @@
         <f t="shared" si="6"/>
         <v>-82077.349999999627</v>
       </c>
-      <c r="O41" s="11">
+      <c r="O41" s="5">
         <f t="shared" si="7"/>
         <v>-1.7099804162586642E-2</v>
       </c>
       <c r="P41">
         <f t="shared" si="8"/>
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -4619,16 +4580,16 @@
         <v>188551675.67999899</v>
       </c>
       <c r="D42">
+        <f t="shared" si="10"/>
+        <v>-41624.320001006126</v>
+      </c>
+      <c r="E42" s="5">
+        <f t="shared" si="2"/>
+        <v>-2.2070943135841053E-4</v>
+      </c>
+      <c r="F42">
         <f t="shared" si="9"/>
-        <v>-41624.320001006126</v>
-      </c>
-      <c r="E42" s="10">
-        <f t="shared" si="10"/>
-        <v>-2.2070943135841053E-4</v>
-      </c>
-      <c r="F42">
-        <f t="shared" si="11"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G42">
         <v>199130300</v>
@@ -4637,16 +4598,16 @@
         <v>196755033.31</v>
       </c>
       <c r="I42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-2375266.6899999976</v>
       </c>
       <c r="J42" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>-1.1928203241796942E-2</v>
       </c>
       <c r="K42">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="L42">
         <v>199954600</v>
@@ -4658,13 +4619,13 @@
         <f t="shared" si="6"/>
         <v>-36.250001013278961</v>
       </c>
-      <c r="O42" s="11">
+      <c r="O42" s="5">
         <f t="shared" si="7"/>
         <v>-1.8129115815929696E-7</v>
       </c>
       <c r="P42">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -4678,16 +4639,16 @@
         <v>7968645.8300000001</v>
       </c>
       <c r="D43">
+        <f t="shared" si="10"/>
+        <v>-166754.16999999993</v>
+      </c>
+      <c r="E43" s="5">
+        <f t="shared" si="2"/>
+        <v>-2.0497353541313264E-2</v>
+      </c>
+      <c r="F43">
         <f t="shared" si="9"/>
-        <v>-166754.16999999993</v>
-      </c>
-      <c r="E43" s="10">
-        <f t="shared" si="10"/>
-        <v>-2.0497353541313264E-2</v>
-      </c>
-      <c r="F43">
-        <f t="shared" si="11"/>
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G43">
         <v>8560800</v>
@@ -4696,16 +4657,16 @@
         <v>8171472.0199999996</v>
       </c>
       <c r="I43">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-389327.98000000045</v>
       </c>
       <c r="J43" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>-4.5477990374731388E-2</v>
       </c>
       <c r="K43">
         <f t="shared" si="5"/>
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="L43">
         <v>8497500</v>
@@ -4717,13 +4678,13 @@
         <f t="shared" si="6"/>
         <v>-346517.43000000995</v>
       </c>
-      <c r="O43" s="11">
+      <c r="O43" s="5">
         <f t="shared" si="7"/>
         <v>-4.0778750220654303E-2</v>
       </c>
       <c r="P43">
         <f t="shared" si="8"/>
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -4737,16 +4698,16 @@
         <v>29789104.379999999</v>
       </c>
       <c r="D44">
+        <f t="shared" si="10"/>
+        <v>-294095.62000000104</v>
+      </c>
+      <c r="E44" s="5">
+        <f t="shared" si="2"/>
+        <v>-9.7760750186150751E-3</v>
+      </c>
+      <c r="F44">
         <f t="shared" si="9"/>
-        <v>-294095.62000000104</v>
-      </c>
-      <c r="E44" s="10">
-        <f t="shared" si="10"/>
-        <v>-9.7760750186150751E-3</v>
-      </c>
-      <c r="F44">
-        <f t="shared" si="11"/>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G44">
         <v>31040700</v>
@@ -4755,16 +4716,16 @@
         <v>30793711.48</v>
       </c>
       <c r="I44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-246988.51999999955</v>
       </c>
       <c r="J44" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>-7.9569249404813532E-3</v>
       </c>
       <c r="K44">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="L44">
         <v>31282200</v>
@@ -4776,13 +4737,13 @@
         <f t="shared" si="6"/>
         <v>-58.75</v>
       </c>
-      <c r="O44" s="11">
+      <c r="O44" s="5">
         <f t="shared" si="7"/>
         <v>-1.8780648419868168E-6</v>
       </c>
       <c r="P44">
         <f t="shared" si="8"/>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -4796,16 +4757,16 @@
         <v>54589584.0499999</v>
       </c>
       <c r="D45">
+        <f t="shared" si="10"/>
+        <v>-712015.95000009984</v>
+      </c>
+      <c r="E45" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.287514194887851E-2</v>
+      </c>
+      <c r="F45">
         <f t="shared" si="9"/>
-        <v>-712015.95000009984</v>
-      </c>
-      <c r="E45" s="10">
-        <f t="shared" si="10"/>
-        <v>-1.287514194887851E-2</v>
-      </c>
-      <c r="F45">
-        <f t="shared" si="11"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G45">
         <v>56792200</v>
@@ -4814,16 +4775,16 @@
         <v>54594953.959999897</v>
       </c>
       <c r="I45">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-2197246.0400001034</v>
       </c>
       <c r="J45" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>-3.8689222111488959E-2</v>
       </c>
       <c r="K45">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="L45">
         <v>56027100</v>
@@ -4835,13 +4796,13 @@
         <f t="shared" si="6"/>
         <v>-640550.34000010043</v>
       </c>
-      <c r="O45" s="11">
+      <c r="O45" s="5">
         <f t="shared" si="7"/>
         <v>-1.1432866237947358E-2</v>
       </c>
       <c r="P45">
         <f t="shared" si="8"/>
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -4855,16 +4816,16 @@
         <v>258322.43</v>
       </c>
       <c r="D46">
+        <f t="shared" si="10"/>
+        <v>-777.57000000000698</v>
+      </c>
+      <c r="E46" s="5">
+        <f t="shared" si="2"/>
+        <v>-3.0010420686993711E-3</v>
+      </c>
+      <c r="F46">
         <f t="shared" si="9"/>
-        <v>-777.57000000000698</v>
-      </c>
-      <c r="E46" s="10">
-        <f t="shared" si="10"/>
-        <v>-3.0010420686993711E-3</v>
-      </c>
-      <c r="F46">
-        <f t="shared" si="11"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G46">
         <v>266000</v>
@@ -4873,16 +4834,16 @@
         <v>257402.90999999901</v>
       </c>
       <c r="I46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-8597.090000000986</v>
       </c>
       <c r="J46" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>-3.2319887218048821E-2</v>
       </c>
       <c r="K46">
         <f t="shared" si="5"/>
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="L46">
         <v>267100</v>
@@ -4894,13 +4855,13 @@
         <f t="shared" si="6"/>
         <v>-12346.840000000986</v>
       </c>
-      <c r="O46" s="11">
+      <c r="O46" s="5">
         <f t="shared" si="7"/>
         <v>-4.6225533508053113E-2</v>
       </c>
       <c r="P46">
         <f t="shared" si="8"/>
-        <v>36</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -4914,16 +4875,16 @@
         <v>70378426.719999999</v>
       </c>
       <c r="D47">
+        <f t="shared" si="10"/>
+        <v>-12273.280000001192</v>
+      </c>
+      <c r="E47" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.7435939690898361E-4</v>
+      </c>
+      <c r="F47">
         <f t="shared" si="9"/>
-        <v>-12273.280000001192</v>
-      </c>
-      <c r="E47" s="10">
-        <f t="shared" si="10"/>
-        <v>-1.7435939690898361E-4</v>
-      </c>
-      <c r="F47">
-        <f t="shared" si="11"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G47">
         <v>73467000</v>
@@ -4932,16 +4893,16 @@
         <v>73442541.659999996</v>
       </c>
       <c r="I47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-24458.340000003576</v>
       </c>
       <c r="J47" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>-3.3291600310348285E-4</v>
       </c>
       <c r="K47">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="L47">
         <v>75072800</v>
@@ -4953,13 +4914,13 @@
         <f t="shared" si="6"/>
         <v>-21970.820000097156</v>
       </c>
-      <c r="O47" s="11">
+      <c r="O47" s="5">
         <f t="shared" si="7"/>
         <v>-2.9266019117572752E-4</v>
       </c>
       <c r="P47">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -4973,16 +4934,16 @@
         <v>6527352.5699999901</v>
       </c>
       <c r="D48">
+        <f t="shared" si="10"/>
+        <v>-209747.43000000995</v>
+      </c>
+      <c r="E48" s="5">
+        <f t="shared" si="2"/>
+        <v>-3.1133192323107857E-2</v>
+      </c>
+      <c r="F48">
         <f t="shared" si="9"/>
-        <v>-209747.43000000995</v>
-      </c>
-      <c r="E48" s="10">
-        <f t="shared" si="10"/>
-        <v>-3.1133192323107857E-2</v>
-      </c>
-      <c r="F48">
-        <f t="shared" si="11"/>
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G48">
         <v>7214700</v>
@@ -4991,16 +4952,16 @@
         <v>6922072.5599999996</v>
       </c>
       <c r="I48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-292627.44000000041</v>
       </c>
       <c r="J48" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>-4.0559890224125802E-2</v>
       </c>
       <c r="K48">
         <f t="shared" si="5"/>
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="L48">
         <v>7289800</v>
@@ -5012,13 +4973,13 @@
         <f t="shared" si="6"/>
         <v>-407449.76000001002</v>
       </c>
-      <c r="O48" s="11">
+      <c r="O48" s="5">
         <f t="shared" si="7"/>
         <v>-5.5893132870587676E-2</v>
       </c>
       <c r="P48">
         <f t="shared" si="8"/>
-        <v>37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -5032,16 +4993,16 @@
         <v>90499.43</v>
       </c>
       <c r="D49">
+        <f t="shared" si="10"/>
+        <v>-1700.570000000007</v>
+      </c>
+      <c r="E49" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.8444360086767971E-2</v>
+      </c>
+      <c r="F49">
         <f t="shared" si="9"/>
-        <v>-1700.570000000007</v>
-      </c>
-      <c r="E49" s="10">
-        <f t="shared" si="10"/>
-        <v>-1.8444360086767971E-2</v>
-      </c>
-      <c r="F49">
-        <f t="shared" si="11"/>
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G49">
         <v>102600</v>
@@ -5050,16 +5011,16 @@
         <v>95466.880000000005</v>
       </c>
       <c r="I49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-7133.1199999999953</v>
       </c>
       <c r="J49" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>-6.9523586744639335E-2</v>
       </c>
       <c r="K49">
         <f t="shared" si="5"/>
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="L49">
         <v>0</v>
@@ -5071,13 +5032,13 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O49" s="11">
+      <c r="O49" s="5">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P49">
+      <c r="P49" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -5091,16 +5052,16 @@
         <v>832600</v>
       </c>
       <c r="D50">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <f>IF(B50&lt;&gt;0, (C50-B50)/B50, "")</f>
+        <v>0</v>
+      </c>
+      <c r="F50" t="b">
         <f t="shared" si="9"/>
         <v>0</v>
-      </c>
-      <c r="E50" s="10">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F50">
-        <f t="shared" si="11"/>
-        <v>2</v>
       </c>
       <c r="G50">
         <v>859100</v>
@@ -5109,16 +5070,16 @@
         <v>859100</v>
       </c>
       <c r="I50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="J50" s="5">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="K50">
+        <f>IF(G50&lt;&gt;0, (H50-G50)/G50, IF(H50=0, " ", ))</f>
+        <v>0</v>
+      </c>
+      <c r="K50" t="b">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L50">
         <v>843200</v>
@@ -5130,13 +5091,13 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O50" s="11">
+      <c r="O50" s="5">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P50">
+      <c r="P50" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -5150,16 +5111,16 @@
         <v>8499425.3399999905</v>
       </c>
       <c r="D51">
+        <f t="shared" si="10"/>
+        <v>-110074.66000000946</v>
+      </c>
+      <c r="E51" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.2785255822058129E-2</v>
+      </c>
+      <c r="F51">
         <f t="shared" si="9"/>
-        <v>-110074.66000000946</v>
-      </c>
-      <c r="E51" s="10">
-        <f t="shared" si="10"/>
-        <v>-1.2785255822058129E-2</v>
-      </c>
-      <c r="F51">
-        <f t="shared" si="11"/>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G51">
         <v>8925500</v>
@@ -5168,16 +5129,16 @@
         <v>8599059.6199999992</v>
       </c>
       <c r="I51">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-326440.38000000082</v>
       </c>
       <c r="J51" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>-3.6573903982970231E-2</v>
       </c>
       <c r="K51">
         <f t="shared" si="5"/>
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="L51">
         <v>8833900</v>
@@ -5189,13 +5150,13 @@
         <f t="shared" si="6"/>
         <v>-98056.689999999478</v>
       </c>
-      <c r="O51" s="11">
+      <c r="O51" s="5">
         <f t="shared" si="7"/>
         <v>-1.1100045280114048E-2</v>
       </c>
       <c r="P51">
         <f t="shared" si="8"/>
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -5209,16 +5170,16 @@
         <v>2254684.7999999998</v>
       </c>
       <c r="D52">
+        <f t="shared" si="10"/>
+        <v>-196315.20000000019</v>
+      </c>
+      <c r="E52" s="5">
+        <f t="shared" si="2"/>
+        <v>-8.009596083231342E-2</v>
+      </c>
+      <c r="F52">
         <f t="shared" si="9"/>
-        <v>-196315.20000000019</v>
-      </c>
-      <c r="E52" s="10">
-        <f t="shared" si="10"/>
-        <v>-8.009596083231342E-2</v>
-      </c>
-      <c r="F52">
-        <f t="shared" si="11"/>
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G52">
         <v>2440700</v>
@@ -5227,16 +5188,16 @@
         <v>2204672.88</v>
       </c>
       <c r="I52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>-236027.12000000011</v>
       </c>
       <c r="J52" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="4"/>
         <v>-9.6704683082722218E-2</v>
       </c>
       <c r="K52">
         <f t="shared" si="5"/>
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="L52">
         <v>2321600</v>
@@ -5248,13 +5209,13 @@
         <f t="shared" si="6"/>
         <v>-264764.74</v>
       </c>
-      <c r="O52" s="11">
+      <c r="O52" s="5">
         <f t="shared" si="7"/>
         <v>-0.11404408166781529</v>
       </c>
       <c r="P52">
         <f t="shared" si="8"/>
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -5289,7 +5250,7 @@
         <v>-27292.159999999974</v>
       </c>
       <c r="D56">
-        <f t="shared" ref="C56:D61" si="14">INDEX($D$1:$N$52, MATCH($A56, $A$1:$A$52, 0), MATCH(D$55, $D$1:$N$1, 0))</f>
+        <f t="shared" ref="C56:D61" si="12">INDEX($D$1:$N$52, MATCH($A56, $A$1:$A$52, 0), MATCH(D$55, $D$1:$N$1, 0))</f>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -5298,15 +5259,15 @@
         <v>25</v>
       </c>
       <c r="B57">
-        <f t="shared" ref="B57:B61" si="15">INDEX($D$1:$N$52, MATCH($A57, $A$1:$A$52, 0), MATCH(B$55, $D$1:$N$1, 0))</f>
+        <f t="shared" ref="B57:B61" si="13">INDEX($D$1:$N$52, MATCH($A57, $A$1:$A$52, 0), MATCH(B$55, $D$1:$N$1, 0))</f>
         <v>0</v>
       </c>
       <c r="C57">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="D57">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -5315,15 +5276,15 @@
         <v>32</v>
       </c>
       <c r="B58">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C58">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D58">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -5332,15 +5293,15 @@
         <v>38</v>
       </c>
       <c r="B59">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -5349,15 +5310,15 @@
         <v>39</v>
       </c>
       <c r="B60">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C60">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D60">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -5366,15 +5327,15 @@
         <v>55</v>
       </c>
       <c r="B61">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C61">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D61">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -5419,15 +5380,15 @@
         <v>25</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B69" si="16">_xlfn.XLOOKUP(A66,$A$1:$A$52,$D$1:$D$52)</f>
+        <f t="shared" ref="B66:B69" si="14">_xlfn.XLOOKUP(A66,$A$1:$A$52,$D$1:$D$52)</f>
         <v>0</v>
       </c>
       <c r="C66">
-        <f t="shared" ref="C66:C70" si="17">_xlfn.XLOOKUP(A66,$A$1:$A$52,$I$1:$I$52)</f>
+        <f t="shared" ref="C66:C70" si="15">_xlfn.XLOOKUP(A66,$A$1:$A$52,$I$1:$I$52)</f>
         <v>0</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D70" si="18">_xlfn.XLOOKUP(A66,$A$1:$A$52,$N$1:$N$52)</f>
+        <f t="shared" ref="D66:D70" si="16">_xlfn.XLOOKUP(A66,$A$1:$A$52,$N$1:$N$52)</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -5436,15 +5397,15 @@
         <v>32</v>
       </c>
       <c r="B67">
+        <f t="shared" si="14"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="15"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D67">
         <f t="shared" si="16"/>
-        <v>-149396.10000000987</v>
-      </c>
-      <c r="C67">
-        <f t="shared" si="17"/>
-        <v>-189254.06000000006</v>
-      </c>
-      <c r="D67">
-        <f t="shared" si="18"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -5453,15 +5414,15 @@
         <v>38</v>
       </c>
       <c r="B68">
+        <f t="shared" si="14"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="15"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D68">
         <f t="shared" si="16"/>
-        <v>-12230.810000000056</v>
-      </c>
-      <c r="C68">
-        <f t="shared" si="17"/>
-        <v>-45485.580000000075</v>
-      </c>
-      <c r="D68">
-        <f t="shared" si="18"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -5470,15 +5431,15 @@
         <v>39</v>
       </c>
       <c r="B69">
+        <f t="shared" si="14"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="15"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D69">
         <f t="shared" si="16"/>
-        <v>-4950.4699999999721</v>
-      </c>
-      <c r="C69">
-        <f t="shared" si="17"/>
-        <v>-8005.7900000010268</v>
-      </c>
-      <c r="D69">
-        <f t="shared" si="18"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -5491,11 +5452,11 @@
         <v>-184239.79000001028</v>
       </c>
       <c r="C70">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D70">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -5540,15 +5501,15 @@
         <v>25</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B79" si="19">INDEX($D$1:$D$52,MATCH(A75,$A$1:$A$52,0))</f>
+        <f t="shared" ref="B75:B79" si="17">INDEX($D$1:$D$52,MATCH(A75,$A$1:$A$52,0))</f>
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" ref="C75:C79" si="20">INDEX($I$1:$I$52,MATCH(A75,$A$1:$A$52,0))</f>
+        <f t="shared" ref="C75:C79" si="18">INDEX($I$1:$I$52,MATCH(A75,$A$1:$A$52,0))</f>
         <v>0</v>
       </c>
       <c r="D75">
-        <f t="shared" ref="D75:D79" si="21">INDEX($N$1:$N$52,MATCH(A75,$A$1:$A$52,0))</f>
+        <f>INDEX($N$1:$N$52,MATCH(A75,$A$1:$A$52,0))</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -5557,15 +5518,15 @@
         <v>32</v>
       </c>
       <c r="B76">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C76">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D76">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="D76:D79" si="19">INDEX($N$1:$N$52,MATCH(A76,$A$1:$A$52,0))</f>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -5574,15 +5535,15 @@
         <v>38</v>
       </c>
       <c r="B77">
+        <f t="shared" si="17"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="18"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D77">
         <f t="shared" si="19"/>
-        <v>-12230.810000000056</v>
-      </c>
-      <c r="C77">
-        <f t="shared" si="20"/>
-        <v>-45485.580000000075</v>
-      </c>
-      <c r="D77">
-        <f t="shared" si="21"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -5591,15 +5552,15 @@
         <v>39</v>
       </c>
       <c r="B78">
+        <f t="shared" si="17"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="18"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D78">
         <f t="shared" si="19"/>
-        <v>-4950.4699999999721</v>
-      </c>
-      <c r="C78">
-        <f t="shared" si="20"/>
-        <v>-8005.7900000010268</v>
-      </c>
-      <c r="D78">
-        <f t="shared" si="21"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -5608,15 +5569,15 @@
         <v>55</v>
       </c>
       <c r="B79">
+        <f t="shared" si="17"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="18"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D79">
         <f t="shared" si="19"/>
-        <v>-184239.79000001028</v>
-      </c>
-      <c r="C79">
-        <f t="shared" si="20"/>
-        <v>-133456.33000001032</v>
-      </c>
-      <c r="D79">
-        <f t="shared" si="21"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -5644,11 +5605,11 @@
       </c>
       <c r="B84" s="6">
         <f>INDEX($B$1:$C$52, MATCH(B87, $A$1:$A$52, 0), 1)</f>
-        <v>14860800</v>
+        <v>356640100</v>
       </c>
       <c r="C84" s="6">
         <f>INDEX($B$1:$C$52, MATCH(B87, $A$1:$A$52, 0), 2)</f>
-        <v>14439480.050000001</v>
+        <v>341243679.13</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -5657,11 +5618,11 @@
       </c>
       <c r="B85" s="6">
         <f>INDEX($G$1:$H$52, MATCH(B87, $A$1:$A$52, 0), 1)</f>
-        <v>15309700</v>
+        <v>382685200</v>
       </c>
       <c r="C85" s="6">
         <f>INDEX($G$1:$H$52, MATCH(B87, $A$1:$A$52, 0), 2)</f>
-        <v>14645233.51</v>
+        <v>346340810.81999999</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -5670,16 +5631,16 @@
       </c>
       <c r="B86" s="6">
         <f>INDEX($L$1:$M$52, MATCH(B87, $A$1:$A$52, 0), 1)</f>
-        <v>15311800</v>
+        <v>376548600</v>
       </c>
       <c r="C86" s="6">
         <f>INDEX($L$1:$M$52, MATCH(B87, $A$1:$A$52, 0), 2)</f>
-        <v>14346057.039999999</v>
+        <v>355279492.22999901</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -5731,7 +5692,7 @@
         <f t="array" ref="B91">_xlfn.XLOOKUP(SMALL(IF($D$2:$D$52&lt;&gt;0, ABS($D$2:$D$52)), 1), IF($D$2:$D$52&lt;&gt;0, ABS($D$2:$D$52)), $A$2:$A$52)</f>
         <v>Register of Deeds</v>
       </c>
-      <c r="C91">
+      <c r="C91" s="5">
         <f>_xlfn.XLOOKUP(B91, $A$2:$A$52, $E$2:$E$52)</f>
         <v>-3.0010420686993711E-3</v>
       </c>
@@ -5739,7 +5700,7 @@
         <f t="array" ref="D91">_xlfn.XLOOKUP(SMALL(IF($D$2:$D$52&lt;&gt;0, ABS($D$2:$D$52)), 2), IF($D$2:$D$52&lt;&gt;0, ABS($D$2:$D$52)), $A$2:$A$52)</f>
         <v>Fire</v>
       </c>
-      <c r="E91">
+      <c r="E91" s="5">
         <f>_xlfn.XLOOKUP(D91, $A$2:$A$52, $E$2:$E$52)</f>
         <v>-1.2379538203300809E-5</v>
       </c>
@@ -5747,7 +5708,7 @@
         <f t="array" ref="F91">_xlfn.XLOOKUP(SMALL(IF($D$2:$D$52&lt;&gt;0, ABS($D$2:$D$52)), 3), IF($D$2:$D$52&lt;&gt;0, ABS($D$2:$D$52)), $A$2:$A$52)</f>
         <v>Soil and Water Conservation</v>
       </c>
-      <c r="G91">
+      <c r="G91" s="5">
         <f>_xlfn.XLOOKUP(F91, $A$2:$A$52, $E$2:$E$52)</f>
         <v>-1.8444360086767971E-2</v>
       </c>
@@ -5760,24 +5721,24 @@
         <f t="array" ref="B92">_xlfn.XLOOKUP(SMALL(IF($I$2:$I$52&lt;&gt;0, ABS($I$2:$I$52)), 1), IF($I$2:$I$52&lt;&gt;0, ABS($I$2:$I$52)), $A$2:$A$52)</f>
         <v>Beer Board</v>
       </c>
-      <c r="C92">
-        <f t="shared" ref="C92:C93" si="22">_xlfn.XLOOKUP(B92, $A$2:$A$52, $E$2:$E$52)</f>
+      <c r="C92" s="5">
+        <f t="shared" ref="C92:C93" si="20">_xlfn.XLOOKUP(B92, $A$2:$A$52, $E$2:$E$52)</f>
         <v>-5.7149963352064452E-2</v>
       </c>
       <c r="D92" t="str" cm="1">
         <f t="array" ref="D92">_xlfn.XLOOKUP(SMALL(IF($I$2:$I$52&lt;&gt;0, ABS($I$2:$I$52)), 2), IF($I$2:$I$52&lt;&gt;0, ABS($I$2:$I$52)), $A$2:$A$52)</f>
         <v>District Attorney</v>
       </c>
-      <c r="E92">
-        <f t="shared" ref="E92:E93" si="23">_xlfn.XLOOKUP(D92, $A$2:$A$52, $E$2:$E$52)</f>
+      <c r="E92" s="5">
+        <f t="shared" ref="E92:E93" si="21">_xlfn.XLOOKUP(D92, $A$2:$A$52, $E$2:$E$52)</f>
         <v>-1.1850188616360429E-2</v>
       </c>
       <c r="F92" t="str" cm="1">
         <f t="array" ref="F92">_xlfn.XLOOKUP(SMALL(IF($I$2:$I$52&lt;&gt;0, ABS($I$2:$I$52)), 3), IF($I$2:$I$52&lt;&gt;0, ABS($I$2:$I$52)), $A$2:$A$52)</f>
         <v>Criminal Justice Planning</v>
       </c>
-      <c r="G92">
-        <f t="shared" ref="G92:G93" si="24">_xlfn.XLOOKUP(F92, $A$2:$A$52, $E$2:$E$52)</f>
+      <c r="G92" s="5">
+        <f t="shared" ref="G92:G93" si="22">_xlfn.XLOOKUP(F92, $A$2:$A$52, $E$2:$E$52)</f>
         <v>-1.3637949218750009E-2</v>
       </c>
     </row>
@@ -5789,24 +5750,24 @@
         <f t="array" ref="B93">_xlfn.XLOOKUP(SMALL(IF($N$2:$N$52&lt;&gt;0, ABS($N$2:$N$52)), 1), IF($N$2:$N$52&lt;&gt;0, ABS($N$2:$N$52)), $A$2:$A$52)</f>
         <v>Justice Integration Services</v>
       </c>
-      <c r="C93">
-        <f t="shared" si="22"/>
+      <c r="C93" s="5">
+        <f t="shared" si="20"/>
         <v>-1.4800253727847622E-2</v>
       </c>
       <c r="D93" t="str" cm="1">
         <f t="array" ref="D93">_xlfn.XLOOKUP(SMALL(IF($N$2:$N$52&lt;&gt;0, ABS($N$2:$N$52)), 2), IF($N$2:$N$52&lt;&gt;0, ABS($N$2:$N$52)), $A$2:$A$52)</f>
         <v>Police</v>
       </c>
-      <c r="E93">
-        <f t="shared" si="23"/>
+      <c r="E93" s="5">
+        <f t="shared" si="21"/>
         <v>-2.2070943135841053E-4</v>
       </c>
       <c r="F93" t="str" cm="1">
         <f t="array" ref="F93">_xlfn.XLOOKUP(SMALL(IF($N$2:$N$52&lt;&gt;0, ABS($N$2:$N$52)), 3), IF($N$2:$N$52&lt;&gt;0, ABS($N$2:$N$52)), $A$2:$A$52)</f>
         <v>Public Library</v>
       </c>
-      <c r="G93">
-        <f t="shared" si="24"/>
+      <c r="G93" s="5">
+        <f t="shared" si="22"/>
         <v>-9.7760750186150751E-3</v>
       </c>
     </row>
@@ -5859,7 +5820,7 @@
         <f t="array" ref="B98">INDEX($A$2:$A$52, MATCH(SMALL(IF($D$2:$D$52&lt;&gt;0, ABS($D$2:$D$52)), 1), IF($D$2:$D$52&lt;&gt;0, ABS($D$2:$D$52)), 0))</f>
         <v>Register of Deeds</v>
       </c>
-      <c r="C98" s="11">
+      <c r="C98" s="5">
         <f>INDEX($E$2:$E$52, MATCH(B98, $A$2:$A$52, 0))</f>
         <v>-3.0010420686993711E-3</v>
       </c>
@@ -5867,7 +5828,7 @@
         <f t="array" ref="D98">INDEX($A$2:$A$52, MATCH(SMALL(IF($D$2:$D$52&lt;&gt;0, ABS($D$2:$D$52)), 2), IF($D$2:$D$52&lt;&gt;0, ABS($D$2:$D$52)), 0))</f>
         <v>Fire</v>
       </c>
-      <c r="E98" s="12">
+      <c r="E98" s="5">
         <f>INDEX($E$2:$E$52, MATCH(D98, $A$2:$A$52, 0))</f>
         <v>-1.2379538203300809E-5</v>
       </c>
@@ -5875,7 +5836,7 @@
         <f t="array" ref="F98">INDEX($A$2:$A$52, MATCH(SMALL(IF($D$2:$D$52&lt;&gt;0, ABS($D$2:$D$52)), 3), IF($D$2:$D$52&lt;&gt;0, ABS($D$2:$D$52)), 0))</f>
         <v>Soil and Water Conservation</v>
       </c>
-      <c r="G98" s="11">
+      <c r="G98" s="5">
         <f>INDEX($E$2:$E$52, MATCH(F98, $A$2:$A$52, 0))</f>
         <v>-1.8444360086767971E-2</v>
       </c>
@@ -5889,7 +5850,7 @@
         <f t="array" ref="B99">INDEX($A$2:$A$52, MATCH(SMALL(IF($I$2:$I$52&lt;&gt;0, ABS($I$2:$I$52)), 1), IF($I$2:$I$52&lt;&gt;0, ABS($I$2:$I$52)), 0))</f>
         <v>Beer Board</v>
       </c>
-      <c r="C99" s="11">
+      <c r="C99" s="5">
         <f>INDEX($J$2:$J$52, MATCH(B99, $A$2:$A$52, 0))</f>
         <v>-1.7301283547257551E-3</v>
       </c>
@@ -5897,7 +5858,7 @@
         <f t="array" ref="D99">INDEX($A$2:$A$52, MATCH(SMALL(IF($I$2:$I$52&lt;&gt;0, ABS($I$2:$I$52)), 2), IF($I$2:$I$52&lt;&gt;0, ABS($I$2:$I$52)), 0))</f>
         <v>District Attorney</v>
       </c>
-      <c r="E99" s="12">
+      <c r="E99" s="5">
         <f>INDEX($J$2:$J$52, MATCH(D99, $A$2:$A$52, 0))</f>
         <v>-2.769017341040361E-4</v>
       </c>
@@ -5905,7 +5866,7 @@
         <f t="array" ref="F99">INDEX($A$2:$A$52, MATCH(SMALL(IF($I$2:$I$52&lt;&gt;0, ABS($I$2:$I$52)), 3), IF($I$2:$I$52&lt;&gt;0, ABS($I$2:$I$52)), 0))</f>
         <v>Criminal Justice Planning</v>
       </c>
-      <c r="G99" s="11">
+      <c r="G99" s="5">
         <f>INDEX($J$2:$J$52, MATCH(F99, $A$2:$A$52, 0))</f>
         <v>-1.1492968897266765E-2</v>
       </c>
@@ -5919,7 +5880,7 @@
         <f t="array" ref="B100">INDEX($A$2:$A$52, MATCH(SMALL(IF($N$2:$N$52&lt;&gt;0, ABS($N$2:$N$52)), 1), IF($N$2:$N$52&lt;&gt;0, ABS($N$2:$N$52)), 0))</f>
         <v>Justice Integration Services</v>
       </c>
-      <c r="C100" s="11">
+      <c r="C100" s="5">
         <f>INDEX($O$2:$O$52, MATCH(B100, $A$2:$A$52, 0))</f>
         <v>-1.2225336516860273E-5</v>
       </c>
@@ -5927,7 +5888,7 @@
         <f t="array" ref="D100">INDEX($A$2:$A$52, MATCH(SMALL(IF($N$2:$N$52&lt;&gt;0, ABS($N$2:$N$52)), 2), IF($N$2:$N$52&lt;&gt;0, ABS($N$2:$N$52)), 0))</f>
         <v>Police</v>
       </c>
-      <c r="E100" s="12">
+      <c r="E100" s="5">
         <f>INDEX($O$2:$O$52, MATCH(D100, $A$2:$A$52, 0))</f>
         <v>-1.8129115815929696E-7</v>
       </c>
@@ -5935,14 +5896,14 @@
         <f t="array" ref="F100">INDEX($A$2:$A$52, MATCH(SMALL(IF($N$2:$N$52&lt;&gt;0, ABS($N$2:$N$52)), 3), IF($N$2:$N$52&lt;&gt;0, ABS($N$2:$N$52)), 0))</f>
         <v>Public Library</v>
       </c>
-      <c r="G100" s="11">
+      <c r="G100" s="5">
         <f>INDEX($O$2:$O$52, MATCH(F100, $A$2:$A$52, 0))</f>
         <v>-1.8780648419868168E-6</v>
       </c>
       <c r="I100" s="4"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B87" xr:uid="{8FD59168-DBA6-4B68-A4C7-3F08B77EA969}">
       <formula1>$A$1:$A$52</formula1>

</xml_diff>